<commit_message>
Added file for comparison between 3 and 4 qubits
</commit_message>
<xml_diff>
--- a/final_eigenvec_four.xlsx
+++ b/final_eigenvec_four.xlsx
@@ -517,802 +517,802 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1</v>
+        <v>7.824700036814042e-23</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.010484013250141e-18</v>
+        <v>-7.90996668856747e-25</v>
       </c>
       <c r="C2" t="n">
-        <v>-5.887136729705683e-09</v>
+        <v>7.909969537698007e-25</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.045576621153476e-18</v>
+        <v>-2.649211851974342e-09</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.313272425290002e-17</v>
+        <v>3.973817138478548e-09</v>
       </c>
       <c r="F2" t="n">
-        <v>3.260194889454067e-31</v>
+        <v>3.386218234753567e-17</v>
       </c>
       <c r="G2" t="n">
-        <v>1.061594882331465e-16</v>
+        <v>9.474734366472908e-17</v>
       </c>
       <c r="H2" t="n">
-        <v>9.381276169191452e-17</v>
+        <v>4.605773699537952e-17</v>
       </c>
       <c r="I2" t="n">
-        <v>-2.185570066388694e-17</v>
+        <v>3.301624516180634e-17</v>
       </c>
       <c r="J2" t="n">
-        <v>3.198064888641693e-17</v>
+        <v>1.410462627063155e-17</v>
       </c>
       <c r="K2" t="n">
-        <v>-4.632620405669542e-26</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>5.111828869385267e-26</v>
+        <v>4.652535058273291e-18</v>
       </c>
       <c r="M2" t="n">
-        <v>-6.531452497401206e-26</v>
+        <v>-4.652532846544745e-18</v>
       </c>
       <c r="N2" t="n">
-        <v>7.304222270942331e-25</v>
+        <v>-3.300154585485897e-09</v>
       </c>
       <c r="O2" t="n">
-        <v>1.470968677080336e-19</v>
+        <v>3.313963346709536e-09</v>
       </c>
       <c r="P2" t="n">
-        <v>1.225358735284193e-17</v>
+        <v>2.483635693623413e-09</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-2.943568364661636e-09</v>
+        <v>-1.323383709164101e-16</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5497768503850368</v>
+        <v>-7.975649896467908e-18</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4999999999999999</v>
+        <v>7.97565192460229e-18</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.4230692742108921</v>
+        <v>1.119538207566623e-16</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.4999999301620939</v>
+        <v>-2.423577456099424e-16</v>
       </c>
       <c r="F3" t="n">
-        <v>1.465460991122025e-16</v>
+        <v>2.838440958027348e-09</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.135376374194462e-08</v>
+        <v>1.51152175241867e-16</v>
       </c>
       <c r="H3" t="n">
-        <v>-7.416264682205347e-09</v>
+        <v>7.574508932552929e-17</v>
       </c>
       <c r="I3" t="n">
-        <v>9.826580875844063e-09</v>
+        <v>1.049000433672486e-09</v>
       </c>
       <c r="J3" t="n">
-        <v>-8.908126577763883e-09</v>
+        <v>5.440030087187521e-09</v>
       </c>
       <c r="K3" t="n">
-        <v>-1.473440169314365e-16</v>
+        <v>4.675079193501772e-09</v>
       </c>
       <c r="L3" t="n">
-        <v>5.406163646024114e-17</v>
+        <v>3.177607318161294e-17</v>
       </c>
       <c r="M3" t="n">
-        <v>-1.654624778273224e-16</v>
+        <v>-3.17760589743568e-17</v>
       </c>
       <c r="N3" t="n">
-        <v>-1.550053947655679e-16</v>
+        <v>0.7059034665040979</v>
       </c>
       <c r="O3" t="n">
-        <v>-2.106253378405731e-09</v>
+        <v>-0.7088571622063429</v>
       </c>
       <c r="P3" t="n">
-        <v>-2.081417018486043e-09</v>
+        <v>-1.700767088962572e-17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-2.943568364661636e-09</v>
+        <v>3.712191947308202e-18</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1319629907052768</v>
+        <v>-5.693259127314406e-18</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4999999999999999</v>
+        <v>5.693260337500187e-18</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2220363309059325</v>
+        <v>2.720025923924078e-16</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8333333573562133</v>
+        <v>-7.591266567732768e-17</v>
       </c>
       <c r="F4" t="n">
-        <v>-6.369610856139844e-16</v>
+        <v>1.848287136065878e-09</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.135376361156931e-08</v>
+        <v>-2.02693863820576e-17</v>
       </c>
       <c r="H4" t="n">
-        <v>-1.460797429478353e-08</v>
+        <v>-1.986908646456741e-09</v>
       </c>
       <c r="I4" t="n">
-        <v>5.110892166897573e-09</v>
+        <v>-2.161579654309105e-17</v>
       </c>
       <c r="J4" t="n">
-        <v>-8.908126810200606e-09</v>
+        <v>-9.234323580264316e-18</v>
       </c>
       <c r="K4" t="n">
-        <v>-5.843789967035725e-17</v>
+        <v>2.483635852652983e-09</v>
       </c>
       <c r="L4" t="n">
-        <v>1.184502632608334e-16</v>
+        <v>-1.873275420810524e-09</v>
       </c>
       <c r="M4" t="n">
-        <v>-7.837595927101519e-17</v>
+        <v>1.873275507322166e-09</v>
       </c>
       <c r="N4" t="n">
-        <v>-6.010546647455957e-18</v>
+        <v>6.356098469985036e-17</v>
       </c>
       <c r="O4" t="n">
-        <v>2.056281115815965e-09</v>
+        <v>-6.382646608192234e-17</v>
       </c>
       <c r="P4" t="n">
-        <v>-2.081417372152791e-09</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-5.443429162602431e-17</v>
+        <v>1.986909167804789e-09</v>
       </c>
       <c r="B5" t="n">
-        <v>7.740313180248157e-09</v>
+        <v>-2.809912852870589e-09</v>
       </c>
       <c r="C5" t="n">
-        <v>1.135376369300663e-08</v>
+        <v>2.80991345529105e-09</v>
       </c>
       <c r="D5" t="n">
-        <v>-7.324376591273696e-09</v>
+        <v>1.015936161921454e-16</v>
       </c>
       <c r="E5" t="n">
-        <v>3.784589010747423e-09</v>
+        <v>2.654952713007304e-16</v>
       </c>
       <c r="F5" t="n">
-        <v>2.156284605739289e-16</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5000000000000001</v>
+        <v>-2.093756012172893e-15</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4980426232847177</v>
+        <v>-1.425667971720675e-15</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.2147155535790062</v>
+        <v>3.947404198563188e-17</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9663872714724742</v>
+        <v>1.602277424961643e-16</v>
       </c>
       <c r="K5" t="n">
-        <v>9.584612655221653e-09</v>
+        <v>-5.172259095606808e-17</v>
       </c>
       <c r="L5" t="n">
-        <v>-8.365282326902203e-09</v>
+        <v>4.822626264909301e-17</v>
       </c>
       <c r="M5" t="n">
-        <v>5.089719410319437e-09</v>
+        <v>-4.822639054643746e-17</v>
       </c>
       <c r="N5" t="n">
-        <v>1.135376380357649e-08</v>
+        <v>-2.003665282216909e-09</v>
       </c>
       <c r="O5" t="n">
-        <v>8.223394147565136e-17</v>
+        <v>2.012049173145372e-09</v>
       </c>
       <c r="P5" t="n">
-        <v>1.25580401379534e-16</v>
+        <v>1.848287108318087e-09</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-2.943568364661636e-09</v>
+        <v>8.947778681589694e-18</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.8141280838709524</v>
+        <v>1.412579647592062e-22</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4999999999999999</v>
+        <v>-1.412131841458648e-22</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2083104728402284</v>
+        <v>9.940058641573251e-16</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1666667270752658</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>2.834785732646204e-16</v>
+        <v>2.914763894239679e-18</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.135376370934402e-08</v>
+        <v>7.947634600841053e-09</v>
       </c>
       <c r="H6" t="n">
-        <v>-1.265029658079973e-08</v>
+        <v>6.623028813236063e-09</v>
       </c>
       <c r="I6" t="n">
-        <v>-5.151643870318592e-09</v>
+        <v>2.630620234079839e-09</v>
       </c>
       <c r="J6" t="n">
-        <v>2.067462016020713e-09</v>
+        <v>-2.370518208077011e-09</v>
       </c>
       <c r="K6" t="n">
-        <v>2.281792988283963e-16</v>
+        <v>-3.973817157781597e-09</v>
       </c>
       <c r="L6" t="n">
-        <v>-1.794070463004428e-16</v>
+        <v>-1.654199140042561e-17</v>
       </c>
       <c r="M6" t="n">
-        <v>2.225201311648758e-16</v>
+        <v>-5.78985487380776e-17</v>
       </c>
       <c r="N6" t="n">
-        <v>6.667679700255705e-17</v>
+        <v>-2.141862327812799e-16</v>
       </c>
       <c r="O6" t="n">
-        <v>-2.106253355584214e-09</v>
+        <v>1.940335268691096e-16</v>
       </c>
       <c r="P6" t="n">
-        <v>-2.08141710695694e-09</v>
+        <v>-2.776684781839089e-17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4.294139945914505e-17</v>
+        <v>1.655756799150126e-09</v>
       </c>
       <c r="B7" t="n">
-        <v>-7.781358989692142e-10</v>
+        <v>-2.319129235922194e-16</v>
       </c>
       <c r="C7" t="n">
-        <v>2.943568363014681e-09</v>
+        <v>2.687905912594896e-16</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.858509460929757e-09</v>
+        <v>-3.70386956391966e-25</v>
       </c>
       <c r="E7" t="n">
-        <v>-1.962378893219821e-09</v>
+        <v>4.675079167707451e-09</v>
       </c>
       <c r="F7" t="n">
-        <v>1.980739549063045e-18</v>
+        <v>-7.002582743014138e-17</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.754898507434523e-16</v>
+        <v>2.024035923506882e-16</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.405861313030631e-16</v>
+        <v>1.703122026984514e-16</v>
       </c>
       <c r="I7" t="n">
-        <v>2.565668411701088e-17</v>
+        <v>-0.5626899833592589</v>
       </c>
       <c r="J7" t="n">
-        <v>-1.381721053832444e-16</v>
+        <v>0.5070541330848104</v>
       </c>
       <c r="K7" t="n">
-        <v>-1.466883595422572e-10</v>
+        <v>-1.857791010823294e-17</v>
       </c>
       <c r="L7" t="n">
-        <v>3.025079110683537e-09</v>
+        <v>3.384738009691889e-16</v>
       </c>
       <c r="M7" t="n">
-        <v>4.197790509521937e-09</v>
+        <v>5.276247773255998e-16</v>
       </c>
       <c r="N7" t="n">
-        <v>-6.113565272897912e-09</v>
+        <v>9.555430008574439e-12</v>
       </c>
       <c r="O7" t="n">
-        <v>0.7155442174736769</v>
+        <v>5.619809096451444e-09</v>
       </c>
       <c r="P7" t="n">
-        <v>0.7071067811865478</v>
+        <v>4.861728531215976e-25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-5.443429162602431e-17</v>
+        <v>1.848287189372453e-09</v>
       </c>
       <c r="B8" t="n">
-        <v>-7.745141292830933e-09</v>
+        <v>2.520148960005804e-18</v>
       </c>
       <c r="C8" t="n">
-        <v>1.13537636930299e-08</v>
+        <v>5.118488226892126e-18</v>
       </c>
       <c r="D8" t="n">
-        <v>-4.886055635239886e-09</v>
+        <v>6.473691970266424e-24</v>
       </c>
       <c r="E8" t="n">
-        <v>7.569174953262493e-09</v>
+        <v>6.623028820918895e-09</v>
       </c>
       <c r="F8" t="n">
-        <v>3.523563091497295e-16</v>
+        <v>-2.258308033597706e-16</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4999999999999996</v>
+        <v>-8.509938411708759e-17</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7885769290754606</v>
+        <v>-1</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.2354340423107633</v>
+        <v>1.440198129235783e-16</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.1817904700076105</v>
+        <v>1.634112224055599e-16</v>
       </c>
       <c r="K8" t="n">
-        <v>-5.326314440107794e-09</v>
+        <v>1.480427496530772e-17</v>
       </c>
       <c r="L8" t="n">
-        <v>2.597922100714651e-09</v>
+        <v>5.61982610430406e-09</v>
       </c>
       <c r="M8" t="n">
-        <v>5.665267422403065e-09</v>
+        <v>5.619826513914061e-09</v>
       </c>
       <c r="N8" t="n">
-        <v>1.135376395275532e-08</v>
+        <v>2.888217771234649e-16</v>
       </c>
       <c r="O8" t="n">
-        <v>-5.78251833466814e-16</v>
+        <v>-2.865149209558429e-16</v>
       </c>
       <c r="P8" t="n">
-        <v>5.792590441993388e-17</v>
+        <v>1.986908646275665e-09</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-9.440133683773771e-25</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>1.932782022392612e-16</v>
+        <v>2.809913475632295e-09</v>
       </c>
       <c r="C9" t="n">
-        <v>1.456182398236846e-16</v>
+        <v>2.809912833901234e-09</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.18412932491051e-17</v>
+        <v>3.313932281341595e-23</v>
       </c>
       <c r="E9" t="n">
-        <v>1.047766452591168e-16</v>
+        <v>-2.895774958993753e-17</v>
       </c>
       <c r="F9" t="n">
-        <v>6.113564979351622e-09</v>
+        <v>-1.986908568650694e-09</v>
       </c>
       <c r="G9" t="n">
-        <v>1.135376369300381e-08</v>
+        <v>-2.886728162108907e-17</v>
       </c>
       <c r="H9" t="n">
-        <v>1.460797433144505e-08</v>
+        <v>1.848287093626292e-09</v>
       </c>
       <c r="I9" t="n">
-        <v>-5.110892099910835e-09</v>
+        <v>9.316779239895282e-10</v>
       </c>
       <c r="J9" t="n">
-        <v>8.90812674515503e-09</v>
+        <v>-8.395586027018407e-10</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.2629488504970353</v>
+        <v>-5.825153784618841e-22</v>
       </c>
       <c r="L9" t="n">
-        <v>0.5713761886872579</v>
+        <v>8.935931456099475e-17</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.2197334032103646</v>
+        <v>-1.113175472854856e-16</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.5000000000000904</v>
+        <v>-2.176516936295965e-16</v>
       </c>
       <c r="O9" t="n">
-        <v>-4.374526466699489e-09</v>
+        <v>2.076513655140275e-16</v>
       </c>
       <c r="P9" t="n">
-        <v>-4.322943315014487e-09</v>
+        <v>-3.672377633393241e-18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-2.943568364661636e-09</v>
+        <v>4.054101869316e-20</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1323882431239241</v>
+        <v>-2.948619879048495e-16</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4999999999999999</v>
+        <v>2.948620914110275e-16</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8534160789917077</v>
+        <v>-1</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1666666956573556</v>
+        <v>4.437151675652741e-16</v>
       </c>
       <c r="F10" t="n">
-        <v>2.768437666391677e-16</v>
+        <v>-3.019015714223487e-18</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.135376370934402e-08</v>
+        <v>3.973817273692584e-09</v>
       </c>
       <c r="H10" t="n">
-        <v>-5.458586706930439e-09</v>
+        <v>5.990407309556648e-18</v>
       </c>
       <c r="I10" t="n">
-        <v>-4.359551364579589e-10</v>
+        <v>-2.433353792460573e-09</v>
       </c>
       <c r="J10" t="n">
-        <v>2.067461858231222e-09</v>
+        <v>-2.537103410996985e-09</v>
       </c>
       <c r="K10" t="n">
-        <v>1.321614641886389e-16</v>
+        <v>-2.649211313002365e-09</v>
       </c>
       <c r="L10" t="n">
-        <v>-1.265582901452958e-16</v>
+        <v>1.756195667610035e-09</v>
       </c>
       <c r="M10" t="n">
-        <v>8.422312996570183e-17</v>
+        <v>-1.756195726033613e-09</v>
       </c>
       <c r="N10" t="n">
-        <v>-1.69120056999864e-16</v>
+        <v>-9.100017487398644e-17</v>
       </c>
       <c r="O10" t="n">
-        <v>2.056281016909838e-09</v>
+        <v>7.481045121215513e-17</v>
       </c>
       <c r="P10" t="n">
-        <v>-2.08141710695694e-09</v>
+        <v>-3.801201230001748e-17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-5.443429162602433e-17</v>
+        <v>4.120744009782603e-16</v>
       </c>
       <c r="B11" t="n">
-        <v>7.745141209185617e-09</v>
+        <v>-2.007080659497989e-09</v>
       </c>
       <c r="C11" t="n">
-        <v>1.135376369302328e-08</v>
+        <v>2.007081081565148e-09</v>
       </c>
       <c r="D11" t="n">
-        <v>4.88605577788022e-09</v>
+        <v>-2.943568364852842e-09</v>
       </c>
       <c r="E11" t="n">
-        <v>-7.56917540997368e-09</v>
+        <v>3.299371215187659e-24</v>
       </c>
       <c r="F11" t="n">
-        <v>7.181221898925965e-17</v>
+        <v>-1.306922109869636e-17</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4999999999999996</v>
+        <v>1.7450977035167e-17</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1551561597283168</v>
+        <v>-2.005011761696782e-16</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.6507754968011135</v>
+        <v>0.8266680002438446</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.1817904670089935</v>
+        <v>0.8619142104186539</v>
       </c>
       <c r="K11" t="n">
-        <v>3.886115479921663e-09</v>
+        <v>-5.366951929102401e-17</v>
       </c>
       <c r="L11" t="n">
-        <v>-1.008745507556252e-09</v>
+        <v>-3.223745476446737e-16</v>
       </c>
       <c r="M11" t="n">
-        <v>-7.695779259550626e-09</v>
+        <v>5.806604262027855e-16</v>
       </c>
       <c r="N11" t="n">
-        <v>1.135376338763458e-08</v>
+        <v>9.555298737089613e-12</v>
       </c>
       <c r="O11" t="n">
-        <v>-3.038486841567748e-16</v>
+        <v>5.6198089657278e-09</v>
       </c>
       <c r="P11" t="n">
-        <v>2.414588146756814e-18</v>
+        <v>1.046948165736032e-24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4.294139945914504e-17</v>
+        <v>2.146244774684155e-16</v>
       </c>
       <c r="B12" t="n">
-        <v>7.781359032891503e-10</v>
+        <v>-1.702977500901151e-09</v>
       </c>
       <c r="C12" t="n">
-        <v>2.943568362581001e-09</v>
+        <v>1.70297783893299e-09</v>
       </c>
       <c r="D12" t="n">
-        <v>1.858509486937103e-09</v>
+        <v>-2.483635807844583e-09</v>
       </c>
       <c r="E12" t="n">
-        <v>1.962378840631404e-09</v>
+        <v>1.86470416435836e-24</v>
       </c>
       <c r="F12" t="n">
-        <v>3.728945011529055e-17</v>
+        <v>-1.821701640826346e-16</v>
       </c>
       <c r="G12" t="n">
-        <v>-1.543973174275919e-16</v>
+        <v>1.213106796442075e-16</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.48439714959738e-16</v>
+        <v>-3.743229428101391e-16</v>
       </c>
       <c r="I12" t="n">
-        <v>7.965649467248128e-17</v>
+        <v>-3.217809688236831e-16</v>
       </c>
       <c r="J12" t="n">
-        <v>-6.279903189938116e-17</v>
+        <v>-2.409134217358464e-16</v>
       </c>
       <c r="K12" t="n">
-        <v>9.221802709530707e-10</v>
+        <v>-6.579676175932491e-18</v>
       </c>
       <c r="L12" t="n">
-        <v>-3.880789614369947e-09</v>
+        <v>-0.7071067724033828</v>
       </c>
       <c r="M12" t="n">
-        <v>-3.104437690175906e-09</v>
+        <v>0.7071067900728011</v>
       </c>
       <c r="N12" t="n">
-        <v>-6.1135649347282e-09</v>
+        <v>-3.096184749165145e-16</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.6985674433009196</v>
+        <v>-3.083263362408814e-16</v>
       </c>
       <c r="P12" t="n">
-        <v>0.7071067811865474</v>
+        <v>2.649211528367558e-09</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-9.440133683773769e-25</v>
+        <v>4.040313890601668e-17</v>
       </c>
       <c r="B13" t="n">
-        <v>4.839399085791521e-16</v>
+        <v>-0.7071067110086425</v>
       </c>
       <c r="C13" t="n">
-        <v>1.456182398253002e-16</v>
+        <v>0.7071068513644451</v>
       </c>
       <c r="D13" t="n">
-        <v>1.02676260287306e-16</v>
+        <v>4.313343468271358e-16</v>
       </c>
       <c r="E13" t="n">
-        <v>4.859331972962081e-17</v>
+        <v>-1.946361808112078e-24</v>
       </c>
       <c r="F13" t="n">
-        <v>6.113565045231692e-09</v>
+        <v>-3.973817292804073e-09</v>
       </c>
       <c r="G13" t="n">
-        <v>1.135376369300381e-08</v>
+        <v>2.188007680662862e-19</v>
       </c>
       <c r="H13" t="n">
-        <v>7.416264655484485e-09</v>
+        <v>-5.732538826621778e-19</v>
       </c>
       <c r="I13" t="n">
-        <v>-9.826580757631556e-09</v>
+        <v>-2.34644844317791e-09</v>
       </c>
       <c r="J13" t="n">
-        <v>8.908126607808597e-09</v>
+        <v>-2.446492450713176e-09</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.581230466291357</v>
+        <v>2.870679841413234e-25</v>
       </c>
       <c r="L13" t="n">
-        <v>0.1654087485682577</v>
+        <v>1.702977630388271e-09</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.2285513545089992</v>
+        <v>-1.702977708783019e-09</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.5000000000001877</v>
+        <v>-6.269234402664087e-17</v>
       </c>
       <c r="O13" t="n">
-        <v>4.270737206387113e-09</v>
+        <v>-7.835519445513556e-17</v>
       </c>
       <c r="P13" t="n">
-        <v>-4.322943315014483e-09</v>
+        <v>-5.673726337629256e-18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-5.443429162602431e-17</v>
+        <v>6.715470931974654e-16</v>
       </c>
       <c r="B14" t="n">
-        <v>-7.740312996525341e-09</v>
+        <v>-1.017640529324797e-17</v>
       </c>
       <c r="C14" t="n">
-        <v>1.135376369302221e-08</v>
+        <v>-1.156542670386365e-17</v>
       </c>
       <c r="D14" t="n">
-        <v>7.324376698010995e-09</v>
+        <v>-3.973817292551323e-09</v>
       </c>
       <c r="E14" t="n">
-        <v>-3.784589170733257e-09</v>
+        <v>7.947634585102668e-09</v>
       </c>
       <c r="F14" t="n">
-        <v>1.19780062211571e-16</v>
+        <v>-2.299588223035076e-15</v>
       </c>
       <c r="G14" t="n">
-        <v>0.4999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="H14" t="n">
-        <v>0.3256171654258309</v>
+        <v>-8.500700718805016e-16</v>
       </c>
       <c r="I14" t="n">
-        <v>0.6891729068497526</v>
+        <v>1.536952353297894e-16</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.0003043929208598285</v>
+        <v>-9.025797794251441e-17</v>
       </c>
       <c r="K14" t="n">
-        <v>-1.102481205477692e-08</v>
+        <v>5.263741594400079e-17</v>
       </c>
       <c r="L14" t="n">
-        <v>9.954458887234535e-09</v>
+        <v>4.68318879815399e-09</v>
       </c>
       <c r="M14" t="n">
-        <v>-7.120232234148582e-09</v>
+        <v>4.683188383694625e-09</v>
       </c>
       <c r="N14" t="n">
-        <v>1.135376344225793e-08</v>
+        <v>2.08495304995301e-09</v>
       </c>
       <c r="O14" t="n">
-        <v>-6.949324648193454e-17</v>
+        <v>2.076252123338593e-09</v>
       </c>
       <c r="P14" t="n">
-        <v>7.874267405190738e-17</v>
+        <v>1.523444410732731e-24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-9.440133683773769e-25</v>
+        <v>8.69903843991277e-18</v>
       </c>
       <c r="B15" t="n">
-        <v>2.726024315960702e-16</v>
+        <v>-1.170797254732926e-09</v>
       </c>
       <c r="C15" t="n">
-        <v>1.456182398236846e-16</v>
+        <v>-1.170797040890147e-09</v>
       </c>
       <c r="D15" t="n">
-        <v>6.822912726511735e-18</v>
+        <v>-1.16972028700551e-17</v>
       </c>
       <c r="E15" t="n">
-        <v>-4.063177544083377e-17</v>
+        <v>2.711370712964966e-17</v>
       </c>
       <c r="F15" t="n">
-        <v>6.113564994875019e-09</v>
+        <v>-6.386081660972935e-19</v>
       </c>
       <c r="G15" t="n">
-        <v>1.13537636930038e-08</v>
+        <v>-2.943568364277768e-09</v>
       </c>
       <c r="H15" t="n">
-        <v>5.458586733736953e-09</v>
+        <v>-1.203193787887785e-18</v>
       </c>
       <c r="I15" t="n">
-        <v>4.359551462647818e-10</v>
+        <v>1.049000622657662e-09</v>
       </c>
       <c r="J15" t="n">
-        <v>-2.067462040046692e-09</v>
+        <v>5.440030157405524e-09</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2389549391594029</v>
+        <v>-9.167840513775201e-26</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.076561943012598</v>
+        <v>7.014040105454907e-17</v>
       </c>
       <c r="M15" t="n">
-        <v>0.9063688557493796</v>
+        <v>-2.584020180877375e-18</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.4999999999999357</v>
+        <v>-0.7083080516113721</v>
       </c>
       <c r="O15" t="n">
-        <v>-4.374526442509172e-09</v>
+        <v>-0.7053520564858163</v>
       </c>
       <c r="P15" t="n">
-        <v>-4.322943315014486e-09</v>
+        <v>4.640120157007941e-33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-9.440133683773768e-25</v>
+        <v>8.730491183095756e-18</v>
       </c>
       <c r="B16" t="n">
-        <v>1.457500082745672e-16</v>
+        <v>-1.702977870764936e-09</v>
       </c>
       <c r="C16" t="n">
-        <v>1.456182398253002e-16</v>
+        <v>-1.702977466731791e-09</v>
       </c>
       <c r="D16" t="n">
-        <v>-1.101575350501728e-16</v>
+        <v>-1.603796174762036e-17</v>
       </c>
       <c r="E16" t="n">
-        <v>7.276250934202733e-17</v>
+        <v>5.263741291526675e-17</v>
       </c>
       <c r="F16" t="n">
-        <v>6.11356507564472e-09</v>
+        <v>-5.117247495282997e-23</v>
       </c>
       <c r="G16" t="n">
-        <v>1.135376369300381e-08</v>
+        <v>-6.623028820918865e-09</v>
       </c>
       <c r="H16" t="n">
-        <v>1.265029649171476e-08</v>
+        <v>-7.947634585102764e-09</v>
       </c>
       <c r="I16" t="n">
-        <v>5.151643912451868e-09</v>
+        <v>-2.920747394811565e-16</v>
       </c>
       <c r="J16" t="n">
-        <v>-2.067462137455105e-09</v>
+        <v>4.124799415372144e-17</v>
       </c>
       <c r="K16" t="n">
-        <v>0.7320721167537699</v>
+        <v>2.418545036754789e-24</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.8001921430384339</v>
+        <v>-0.707106789969712</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.2792436341141071</v>
+        <v>-0.7071067723002938</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.4999999999997854</v>
+        <v>-1.720297383699401e-17</v>
       </c>
       <c r="O16" t="n">
-        <v>4.270737239840962e-09</v>
+        <v>-1.713118541548484e-17</v>
       </c>
       <c r="P16" t="n">
-        <v>-4.322943315014483e-09</v>
+        <v>-1.228206301356223e-17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-1.85545208219149e-33</v>
+        <v>3.973817292551331e-09</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.870659472296648e-16</v>
+        <v>-0.7071068513644454</v>
       </c>
       <c r="C17" t="n">
-        <v>-4.044797641107851e-21</v>
+        <v>-0.707106711008643</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.796382976598059e-16</v>
+        <v>-3.207658800987072e-23</v>
       </c>
       <c r="E17" t="n">
-        <v>4.040960745649118e-16</v>
+        <v>-3.668979670910397e-25</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2.36868352585634e-17</v>
       </c>
       <c r="G17" t="n">
-        <v>-5.795703188411077e-16</v>
+        <v>3.620562805373819e-17</v>
       </c>
       <c r="H17" t="n">
-        <v>-5.496601842386342e-16</v>
+        <v>2.107625470069782e-17</v>
       </c>
       <c r="I17" t="n">
-        <v>1.708822187603337e-16</v>
+        <v>-1.179710779764038e-16</v>
       </c>
       <c r="J17" t="n">
-        <v>-4.990392424653443e-16</v>
+        <v>-1.802916187810417e-16</v>
       </c>
       <c r="K17" t="n">
-        <v>-7.754919187119691e-10</v>
+        <v>-1.891876555947446e-30</v>
       </c>
       <c r="L17" t="n">
-        <v>8.557105258783856e-10</v>
+        <v>1.702977690718497e-09</v>
       </c>
       <c r="M17" t="n">
-        <v>-1.093352826873097e-09</v>
+        <v>1.702977648163928e-09</v>
       </c>
       <c r="N17" t="n">
-        <v>1.222712993751802e-08</v>
+        <v>1.172786159977733e-09</v>
       </c>
       <c r="O17" t="n">
-        <v>6.102544563563982e-17</v>
+        <v>1.167891749749972e-09</v>
       </c>
       <c r="P17" t="n">
-        <v>5.326319502923056e-17</v>
+        <v>2.728456634007237e-26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Five and four qubits
Advantage + KP values for the parameters
</commit_message>
<xml_diff>
--- a/final_eigenvec_four.xlsx
+++ b/final_eigenvec_four.xlsx
@@ -517,802 +517,802 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-4.791395215317022e-17</v>
+        <v>-1.036232854677933e-22</v>
       </c>
       <c r="B2" t="n">
-        <v>1.404956545228357e-09</v>
+        <v>-1.681332379119761e-32</v>
       </c>
       <c r="C2" t="n">
-        <v>2.486794716549161e-17</v>
+        <v>-8.166549349893839e-23</v>
       </c>
       <c r="D2" t="n">
-        <v>1.40495658321057e-09</v>
+        <v>8.166690288005269e-23</v>
       </c>
       <c r="E2" t="n">
-        <v>1.869465055915054e-17</v>
+        <v>3.111256778370345e-33</v>
       </c>
       <c r="F2" t="n">
-        <v>-2.649211651567455e-09</v>
+        <v>-4.617119692812142e-33</v>
       </c>
       <c r="G2" t="n">
-        <v>1.901788124646647e-17</v>
+        <v>4.6171028718429e-33</v>
       </c>
       <c r="H2" t="n">
-        <v>1.265527664141256e-16</v>
+        <v>2.71564472260426e-22</v>
       </c>
       <c r="I2" t="n">
-        <v>-2.037087085778701e-24</v>
+        <v>-4.658119932132633e-22</v>
       </c>
       <c r="J2" t="n">
-        <v>4.930565902337734e-08</v>
+        <v>8.042144018329229e-23</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.256995581815582e-06</v>
+        <v>3.996898153757778e-22</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.9999999999999936</v>
+        <v>9.657171269114655e-12</v>
       </c>
       <c r="M2" t="n">
-        <v>-4.97929878890906e-08</v>
+        <v>1.016544344117341e-11</v>
       </c>
       <c r="N2" t="n">
-        <v>-5.61982454981043e-09</v>
+        <v>1.073019029901643e-11</v>
       </c>
       <c r="O2" t="n">
-        <v>7.947634816675278e-09</v>
+        <v>1.136137796366431e-11</v>
       </c>
       <c r="P2" t="n">
-        <v>5.619828789389698e-09</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-8.454945799986349e-17</v>
+        <v>-1.07301896317416e-11</v>
       </c>
       <c r="B3" t="n">
-        <v>8.388092710014329e-18</v>
+        <v>-1.93495569359993e-21</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.123965272138218e-09</v>
+        <v>7.066125231047504e-18</v>
       </c>
       <c r="D3" t="n">
-        <v>4.37384431754424e-17</v>
+        <v>-7.067056197319154e-18</v>
       </c>
       <c r="E3" t="n">
-        <v>1.123965021541687e-09</v>
+        <v>4.002330981565128e-22</v>
       </c>
       <c r="F3" t="n">
-        <v>1.088282930255089e-16</v>
+        <v>-1.777411577244597e-22</v>
       </c>
       <c r="G3" t="n">
-        <v>-3.990518032314929e-17</v>
+        <v>-1.596100714375952e-22</v>
       </c>
       <c r="H3" t="n">
-        <v>-2.649211487210445e-09</v>
+        <v>2.146041825515863e-11</v>
       </c>
       <c r="I3" t="n">
-        <v>4.438354023504441e-17</v>
+        <v>-2.154232952819525e-11</v>
       </c>
       <c r="J3" t="n">
-        <v>5.619826443550545e-09</v>
+        <v>2.234731249473008e-11</v>
       </c>
       <c r="K3" t="n">
-        <v>-2.593157034368535e-14</v>
+        <v>1.631888509184236e-17</v>
       </c>
       <c r="L3" t="n">
-        <v>-7.947634622023717e-09</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>5.619825876921995e-09</v>
+        <v>5.994110713235593e-15</v>
       </c>
       <c r="N3" t="n">
-        <v>1.519013210400923e-08</v>
+        <v>6.660187513674559e-16</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.9999999999999998</v>
+        <v>-4.043647085677147e-16</v>
       </c>
       <c r="P3" t="n">
-        <v>-2.084486656118879e-08</v>
+        <v>-9.656940896947432e-12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.78984338190663e-16</v>
+        <v>9.117503425189895e-18</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7071067607900842</v>
+        <v>-1.29335736330914e-23</v>
       </c>
       <c r="C4" t="n">
-        <v>1.476382933709643e-08</v>
+        <v>-7.187995025634125e-12</v>
       </c>
       <c r="D4" t="n">
-        <v>0.707106788336059</v>
+        <v>7.188119076300633e-12</v>
       </c>
       <c r="E4" t="n">
-        <v>7.16098279175738e-09</v>
+        <v>-1.11106675629875e-21</v>
       </c>
       <c r="F4" t="n">
-        <v>-4.458992102078167e-16</v>
+        <v>-8.729270386699821e-22</v>
       </c>
       <c r="G4" t="n">
-        <v>-7.947634304397499e-09</v>
+        <v>4.928775308882372e-22</v>
       </c>
       <c r="H4" t="n">
-        <v>1.036287043637474e-16</v>
+        <v>2.443626581453735e-17</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.779737839926111e-16</v>
+        <v>-1.50796173660397e-11</v>
       </c>
       <c r="J4" t="n">
-        <v>-1.404956631899365e-09</v>
+        <v>1.564309955763869e-11</v>
       </c>
       <c r="K4" t="n">
-        <v>6.365650487629501e-15</v>
+        <v>2.414294852692855e-11</v>
       </c>
       <c r="L4" t="n">
-        <v>1.986908667264883e-09</v>
+        <v>5.941540696923834e-17</v>
       </c>
       <c r="M4" t="n">
-        <v>-1.404956611352204e-09</v>
+        <v>6.106718605282241e-16</v>
       </c>
       <c r="N4" t="n">
-        <v>8.945089985647079e-17</v>
+        <v>1.339266608542708e-15</v>
       </c>
       <c r="O4" t="n">
-        <v>1.445902487406277e-17</v>
+        <v>1</v>
       </c>
       <c r="P4" t="n">
-        <v>1.413339823982785e-16</v>
+        <v>-1.136173316801328e-11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-1.589527007195798e-09</v>
+        <v>-1.110568744945022e-16</v>
       </c>
       <c r="B5" t="n">
-        <v>1.404956469671912e-09</v>
+        <v>2.931721386475353e-17</v>
       </c>
       <c r="C5" t="n">
-        <v>3.826725183991351e-17</v>
+        <v>-1.517449074881796e-11</v>
       </c>
       <c r="D5" t="n">
-        <v>1.404956430495931e-09</v>
+        <v>-1.51748937261747e-11</v>
       </c>
       <c r="E5" t="n">
-        <v>5.295347273548681e-18</v>
+        <v>-2.414323856242113e-11</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.227964713682291e-16</v>
+        <v>-1.211193598966174e-16</v>
       </c>
       <c r="G5" t="n">
-        <v>-8.934717583481916e-17</v>
+        <v>1.211050210022838e-16</v>
       </c>
       <c r="H5" t="n">
-        <v>-2.190997614390188e-16</v>
+        <v>2.195917947110037e-16</v>
       </c>
       <c r="I5" t="n">
-        <v>-5.263739448628545e-18</v>
+        <v>-0.7807480474653604</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7071067645711594</v>
+        <v>0.8099215765986721</v>
       </c>
       <c r="K5" t="n">
-        <v>-5.924296026261987e-09</v>
+        <v>6.122626597949276e-17</v>
       </c>
       <c r="L5" t="n">
-        <v>-1.056375345529552e-08</v>
+        <v>-2.759176053385392e-11</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7071067646438756</v>
+        <v>-1.574023087392656e-16</v>
       </c>
       <c r="N5" t="n">
-        <v>-2.6721091769479e-16</v>
+        <v>-8.995716286418389e-17</v>
       </c>
       <c r="O5" t="n">
-        <v>7.947634289242354e-09</v>
+        <v>-1.931424581946772e-11</v>
       </c>
       <c r="P5" t="n">
-        <v>3.869632969016533e-16</v>
+        <v>1.503558541149491e-22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4.49802097544373e-16</v>
+        <v>-9.657188836838101e-12</v>
       </c>
       <c r="B6" t="n">
-        <v>5.619825996399492e-09</v>
+        <v>-1.756118195063036e-21</v>
       </c>
       <c r="C6" t="n">
-        <v>8.607249544361263e-17</v>
+        <v>1.319085049485686e-17</v>
       </c>
       <c r="D6" t="n">
-        <v>-5.619826741797403e-09</v>
+        <v>-1.319118218817301e-17</v>
       </c>
       <c r="E6" t="n">
-        <v>-8.817790211136126e-17</v>
+        <v>1.683647746509007e-21</v>
       </c>
       <c r="F6" t="n">
-        <v>-1</v>
+        <v>7.799659062309739e-22</v>
       </c>
       <c r="G6" t="n">
-        <v>1.817254671520777e-08</v>
+        <v>-3.572209909903872e-22</v>
       </c>
       <c r="H6" t="n">
-        <v>7.947634599448367e-09</v>
+        <v>-1.121540905332171e-17</v>
       </c>
       <c r="I6" t="n">
-        <v>-1.303845808312724e-16</v>
+        <v>-1.34094410500141e-11</v>
       </c>
       <c r="J6" t="n">
-        <v>-8.55789526660135e-17</v>
+        <v>-1.258732465393586e-11</v>
       </c>
       <c r="K6" t="n">
-        <v>8.64426112286507e-15</v>
+        <v>2.759189352235694e-11</v>
       </c>
       <c r="L6" t="n">
-        <v>2.649211422964647e-09</v>
+        <v>-6.213372908313923e-16</v>
       </c>
       <c r="M6" t="n">
-        <v>1.661857528360791e-16</v>
+        <v>-4.089820745680538e-15</v>
       </c>
       <c r="N6" t="n">
-        <v>-1.404956900575475e-09</v>
+        <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>-1.29332040735327e-16</v>
+        <v>-3.056582764667324e-15</v>
       </c>
       <c r="P6" t="n">
-        <v>-1.404956276402008e-09</v>
+        <v>-1.07286927637977e-11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-3.490925347333293e-16</v>
+        <v>-1</v>
       </c>
       <c r="B7" t="n">
-        <v>1.848809969166109e-16</v>
+        <v>-1.931434256379727e-10</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.80991282165652e-09</v>
+        <v>-2.79145909033353e-16</v>
       </c>
       <c r="D7" t="n">
-        <v>4.269119686960082e-16</v>
+        <v>2.830006589978719e-16</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.809913486223634e-09</v>
+        <v>6.43811430059132e-11</v>
       </c>
       <c r="F7" t="n">
-        <v>-7.947634585100525e-09</v>
+        <v>-1.51324093306471e-18</v>
       </c>
       <c r="G7" t="n">
-        <v>1.449772383312318e-16</v>
+        <v>1.530787023740159e-18</v>
       </c>
       <c r="H7" t="n">
-        <v>-1</v>
+        <v>1.401137829263262e-16</v>
       </c>
       <c r="I7" t="n">
-        <v>1.640545747595641e-08</v>
+        <v>-2.554728460056816e-16</v>
       </c>
       <c r="J7" t="n">
-        <v>-2.809914026368607e-09</v>
+        <v>5.35963860758549e-17</v>
       </c>
       <c r="K7" t="n">
-        <v>-1.684294707444037e-21</v>
+        <v>7.722582432092188e-17</v>
       </c>
       <c r="L7" t="n">
-        <v>-4.85479363280188e-16</v>
+        <v>-1.073019029903051e-11</v>
       </c>
       <c r="M7" t="n">
-        <v>2.809913281335615e-09</v>
+        <v>3.760756258047686e-23</v>
       </c>
       <c r="N7" t="n">
-        <v>1.090582022258743e-16</v>
+        <v>-9.6571712691485e-12</v>
       </c>
       <c r="O7" t="n">
-        <v>2.649211627660587e-09</v>
+        <v>1.022041877917098e-23</v>
       </c>
       <c r="P7" t="n">
-        <v>6.410096261001015e-17</v>
+        <v>1.036063555944485e-22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-7.143948476214803e-16</v>
+        <v>1.532980422344469e-16</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7071068015830101</v>
+        <v>-7.593513408075343e-19</v>
       </c>
       <c r="C8" t="n">
-        <v>1.476383036962401e-08</v>
+        <v>-9.151184712442485e-17</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.707106774037036</v>
+        <v>9.327291057562296e-17</v>
       </c>
       <c r="E8" t="n">
-        <v>-7.160981536667375e-09</v>
+        <v>-1.931440674250336e-11</v>
       </c>
       <c r="F8" t="n">
-        <v>7.947634585102651e-09</v>
+        <v>1.517480723843754e-11</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.138732629052203e-16</v>
+        <v>-1.517475196535439e-11</v>
       </c>
       <c r="H8" t="n">
-        <v>-2.505895409154678e-16</v>
+        <v>-3.951529720224298e-17</v>
       </c>
       <c r="I8" t="n">
-        <v>2.475651866878638e-16</v>
+        <v>-1.085148659835906e-16</v>
       </c>
       <c r="J8" t="n">
-        <v>-1.404956685741631e-09</v>
+        <v>2.057559085583267e-16</v>
       </c>
       <c r="K8" t="n">
-        <v>1.986908420805276e-09</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>-2.330085690351225e-16</v>
+        <v>-7.034652372932426e-19</v>
       </c>
       <c r="M8" t="n">
-        <v>1.404956812368665e-09</v>
+        <v>4.285286258340713e-19</v>
       </c>
       <c r="N8" t="n">
-        <v>-1.858129007142997e-17</v>
+        <v>-2.759191801217852e-11</v>
       </c>
       <c r="O8" t="n">
-        <v>-1.25434227781537e-17</v>
+        <v>-2.414292816397255e-11</v>
       </c>
       <c r="P8" t="n">
-        <v>-8.422073074254999e-19</v>
+        <v>1.706409072799458e-22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-3.524669783313165e-17</v>
+        <v>-6.438079788469179e-11</v>
       </c>
       <c r="B9" t="n">
-        <v>1.404956304170656e-09</v>
+        <v>-1.541994180325995e-15</v>
       </c>
       <c r="C9" t="n">
-        <v>4.444550814274301e-17</v>
+        <v>-5.441272745586317e-16</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.404956488699788e-09</v>
+        <v>1.864211858351288e-15</v>
       </c>
       <c r="E9" t="n">
-        <v>-4.699675280774296e-17</v>
+        <v>-1</v>
       </c>
       <c r="F9" t="n">
-        <v>-3.288472509412399e-25</v>
+        <v>-1.365703965208477e-10</v>
       </c>
       <c r="G9" t="n">
-        <v>4.20350862210951e-16</v>
+        <v>-1.365756551291545e-10</v>
       </c>
       <c r="H9" t="n">
-        <v>-3.973817509142579e-09</v>
+        <v>6.51289742165428e-17</v>
       </c>
       <c r="I9" t="n">
-        <v>-3.973817227428856e-09</v>
+        <v>1.884941967829163e-11</v>
       </c>
       <c r="J9" t="n">
-        <v>0.7071067978019335</v>
+        <v>-1.955375358015932e-11</v>
       </c>
       <c r="K9" t="n">
-        <v>3.668873807886259e-13</v>
+        <v>-1.931427712973458e-11</v>
       </c>
       <c r="L9" t="n">
-        <v>1.126357801706501e-07</v>
+        <v>4.933582038967252e-22</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.7071067977292174</v>
+        <v>1.481658855806176e-25</v>
       </c>
       <c r="N9" t="n">
-        <v>-1.405997616300127e-16</v>
+        <v>4.231201798904439e-22</v>
       </c>
       <c r="O9" t="n">
-        <v>-2.405758192412731e-16</v>
+        <v>4.663175341856139e-22</v>
       </c>
       <c r="P9" t="n">
-        <v>8.052095395285393e-17</v>
+        <v>-2.342812185182386e-33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-1.244977741761643e-17</v>
+        <v>7.782943328115727e-18</v>
       </c>
       <c r="B10" t="n">
-        <v>1.375567645816195e-16</v>
+        <v>4.831206747893899e-22</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.123965515471726e-09</v>
+        <v>-8.033655272116433e-12</v>
       </c>
       <c r="D10" t="n">
-        <v>-4.704702427151805e-17</v>
+        <v>8.033793917072827e-12</v>
       </c>
       <c r="E10" t="n">
-        <v>1.123965239774304e-09</v>
+        <v>-4.089991652730208e-22</v>
       </c>
       <c r="F10" t="n">
-        <v>1.021476442283426e-16</v>
+        <v>-5.420738390863429e-22</v>
       </c>
       <c r="G10" t="n">
-        <v>1.986908686180845e-09</v>
+        <v>8.367266997640653e-22</v>
       </c>
       <c r="H10" t="n">
-        <v>-7.798233203980116e-17</v>
+        <v>1.931429166024468e-11</v>
       </c>
       <c r="I10" t="n">
-        <v>-9.220123049782202e-19</v>
+        <v>-1.508562958748424e-11</v>
       </c>
       <c r="J10" t="n">
-        <v>4.997490841598563e-16</v>
+        <v>-1.416077417627182e-11</v>
       </c>
       <c r="K10" t="n">
-        <v>-2.592844481193889e-14</v>
+        <v>-1.228362757152175e-17</v>
       </c>
       <c r="L10" t="n">
-        <v>-7.947634517456577e-09</v>
+        <v>-5.513015296897995e-15</v>
       </c>
       <c r="M10" t="n">
-        <v>-4.839550258933788e-16</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
-        <v>0.7071066649607298</v>
+        <v>5.567700535660178e-15</v>
       </c>
       <c r="O10" t="n">
-        <v>1.715901772269882e-08</v>
+        <v>-1.198007077412873e-15</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.7071068978278831</v>
+        <v>-1.016482316582114e-11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-7.947634485527637e-09</v>
+        <v>7.422668723844378e-17</v>
       </c>
       <c r="B11" t="n">
-        <v>2.247930421393511e-09</v>
+        <v>2.414292984068295e-11</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.7071068633249975</v>
+        <v>-1.951051822093606e-11</v>
       </c>
       <c r="D11" t="n">
-        <v>2.247930626345625e-09</v>
+        <v>-1.951033888895094e-11</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7071066994604446</v>
+        <v>7.132816766766335e-17</v>
       </c>
       <c r="F11" t="n">
-        <v>-1.576338590947901e-24</v>
+        <v>-1.274664482070851e-18</v>
       </c>
       <c r="G11" t="n">
-        <v>6.494153867164365e-17</v>
+        <v>1.266471142440308e-18</v>
       </c>
       <c r="H11" t="n">
-        <v>-5.263729112975938e-18</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>-7.205905933449735e-17</v>
+        <v>8.586242091546045e-17</v>
       </c>
       <c r="J11" t="n">
-        <v>-3.954550450366526e-17</v>
+        <v>7.927753658747034e-17</v>
       </c>
       <c r="K11" t="n">
-        <v>-9.645667907105946e-17</v>
+        <v>-1.47451497343439e-17</v>
       </c>
       <c r="L11" t="n">
-        <v>3.158244383158837e-17</v>
+        <v>-2.146024322006007e-11</v>
       </c>
       <c r="M11" t="n">
-        <v>2.16797604274424e-17</v>
+        <v>-1.931443291938531e-11</v>
       </c>
       <c r="N11" t="n">
-        <v>-1.123964978538765e-09</v>
+        <v>2.24637446287797e-17</v>
       </c>
       <c r="O11" t="n">
-        <v>1.589527063363281e-09</v>
+        <v>-2.065563270140633e-18</v>
       </c>
       <c r="P11" t="n">
-        <v>1.123965357675678e-09</v>
+        <v>1.320040313855912e-22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-3.97381729681501e-09</v>
+        <v>1.600739220577689e-16</v>
       </c>
       <c r="B12" t="n">
-        <v>5.619825802728809e-09</v>
+        <v>-2.522237112090684e-15</v>
       </c>
       <c r="C12" t="n">
-        <v>2.618900175957362e-17</v>
+        <v>-0.7071006793750427</v>
       </c>
       <c r="D12" t="n">
-        <v>5.619826075849044e-09</v>
+        <v>0.7071128825524579</v>
       </c>
       <c r="E12" t="n">
-        <v>1.847326779093311e-16</v>
+        <v>7.044424980886948e-17</v>
       </c>
       <c r="F12" t="n">
-        <v>5.960725938827003e-09</v>
+        <v>-6.828663451425932e-11</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9999999999999998</v>
+        <v>6.828638575721117e-11</v>
       </c>
       <c r="H12" t="n">
-        <v>6.015784396463383e-19</v>
+        <v>-4.906190289695546e-16</v>
       </c>
       <c r="I12" t="n">
-        <v>8.225658080984939e-18</v>
+        <v>-2.300957280430481e-16</v>
       </c>
       <c r="J12" t="n">
-        <v>8.942447908619636e-17</v>
+        <v>3.488532565669355e-17</v>
       </c>
       <c r="K12" t="n">
-        <v>2.64921152332841e-09</v>
+        <v>-1.937106113283201e-17</v>
       </c>
       <c r="L12" t="n">
-        <v>-4.056888780807317e-17</v>
+        <v>2.106310406990328e-24</v>
       </c>
       <c r="M12" t="n">
-        <v>-1.962114644151264e-16</v>
+        <v>-1.136137796367196e-11</v>
       </c>
       <c r="N12" t="n">
-        <v>-1.404956313056402e-09</v>
+        <v>8.442281831172406e-24</v>
       </c>
       <c r="O12" t="n">
-        <v>1.28833309784653e-18</v>
+        <v>-1.016544344117642e-11</v>
       </c>
       <c r="P12" t="n">
-        <v>1.404956792491279e-09</v>
+        <v>1.154900087443605e-22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-1</v>
+        <v>-2.004483291426057e-25</v>
       </c>
       <c r="B13" t="n">
-        <v>1.838010907787526e-16</v>
+        <v>4.734144518475036e-15</v>
       </c>
       <c r="C13" t="n">
-        <v>5.619827226964997e-09</v>
+        <v>-0.7071128829453985</v>
       </c>
       <c r="D13" t="n">
-        <v>4.589048309835845e-16</v>
+        <v>-0.7071006797679902</v>
       </c>
       <c r="E13" t="n">
-        <v>-5.619825794586185e-09</v>
+        <v>-1.923134077490348e-16</v>
       </c>
       <c r="F13" t="n">
-        <v>-3.059032693761447e-17</v>
+        <v>-6.828645794206624e-11</v>
       </c>
       <c r="G13" t="n">
-        <v>-3.973817289104696e-09</v>
+        <v>-6.828656788795495e-11</v>
       </c>
       <c r="H13" t="n">
-        <v>1.782709886200442e-16</v>
+        <v>-2.759191791175646e-11</v>
       </c>
       <c r="I13" t="n">
-        <v>2.64921152814889e-09</v>
+        <v>1.675503192581534e-11</v>
       </c>
       <c r="J13" t="n">
-        <v>-1.123965153295244e-09</v>
+        <v>-1.738122816398455e-11</v>
       </c>
       <c r="K13" t="n">
-        <v>-1.315972757743197e-18</v>
+        <v>-2.182431025882176e-25</v>
       </c>
       <c r="L13" t="n">
-        <v>1.089285086805521e-16</v>
+        <v>5.921275742077835e-22</v>
       </c>
       <c r="M13" t="n">
-        <v>-1.123965203485593e-09</v>
+        <v>3.485224005666194e-22</v>
       </c>
       <c r="N13" t="n">
-        <v>2.107873112338342e-16</v>
+        <v>4.35120607344181e-28</v>
       </c>
       <c r="O13" t="n">
-        <v>2.808732687026924e-16</v>
+        <v>2.996742145423013e-22</v>
       </c>
       <c r="P13" t="n">
-        <v>-2.107873807562135e-16</v>
+        <v>-2.13436292205868e-33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3.231764690688054e-19</v>
+        <v>6.37286102559884e-17</v>
       </c>
       <c r="B14" t="n">
-        <v>-3.839469278182398e-17</v>
+        <v>1.931421085411896e-11</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.123965131342471e-09</v>
+        <v>3.562859036743195e-16</v>
       </c>
       <c r="D14" t="n">
-        <v>1.291757161534017e-16</v>
+        <v>1.720734678578681e-17</v>
       </c>
       <c r="E14" t="n">
-        <v>-1.123965391809593e-09</v>
+        <v>-1.705925861010295e-16</v>
       </c>
       <c r="F14" t="n">
-        <v>-1.986908542172475e-09</v>
+        <v>1.951046815470161e-11</v>
       </c>
       <c r="G14" t="n">
-        <v>4.53187352560441e-17</v>
+        <v>-1.951039708355994e-11</v>
       </c>
       <c r="H14" t="n">
-        <v>2.354504517120127e-17</v>
+        <v>1.544619257860951e-16</v>
       </c>
       <c r="I14" t="n">
-        <v>2.847305847370812e-25</v>
+        <v>-0.6248459701230595</v>
       </c>
       <c r="J14" t="n">
-        <v>1.2339068844573e-16</v>
+        <v>-0.5865381826956547</v>
       </c>
       <c r="K14" t="n">
-        <v>-7.947634585058457e-09</v>
+        <v>1.672549891932644e-16</v>
       </c>
       <c r="L14" t="n">
-        <v>6.334637599702184e-16</v>
+        <v>-8.869756629800233e-25</v>
       </c>
       <c r="M14" t="n">
-        <v>4.461485254348699e-17</v>
+        <v>-2.414292817278483e-11</v>
       </c>
       <c r="N14" t="n">
-        <v>0.7071068974123458</v>
+        <v>-2.14603805980339e-11</v>
       </c>
       <c r="O14" t="n">
-        <v>1.421962020776973e-08</v>
+        <v>2.579890704434267e-25</v>
       </c>
       <c r="P14" t="n">
-        <v>0.7071066645451922</v>
+        <v>1.49428971361494e-22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-8.421986084553753e-17</v>
+        <v>-1.931434253822939e-10</v>
       </c>
       <c r="B15" t="n">
-        <v>2.247930627165379e-09</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.7071066990480878</v>
+        <v>9.226093206815878e-16</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.247930515287396e-09</v>
+        <v>4.078367769298119e-15</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.707106862912641</v>
+        <v>-1.12611528290278e-15</v>
       </c>
       <c r="F15" t="n">
-        <v>7.895611934536179e-17</v>
+        <v>-4.552476976591992e-11</v>
       </c>
       <c r="G15" t="n">
-        <v>4.035957284794561e-22</v>
+        <v>-4.552391412263053e-11</v>
       </c>
       <c r="H15" t="n">
-        <v>3.973817292551335e-09</v>
+        <v>-2.414292817278628e-11</v>
       </c>
       <c r="I15" t="n">
-        <v>3.97381723331277e-09</v>
+        <v>1.206842813504288e-11</v>
       </c>
       <c r="J15" t="n">
-        <v>1.11660847554646e-17</v>
+        <v>1.132854215111745e-11</v>
       </c>
       <c r="K15" t="n">
-        <v>2.523682677619676e-17</v>
+        <v>2.844064444401423e-25</v>
       </c>
       <c r="L15" t="n">
-        <v>1.407545335300228e-24</v>
+        <v>3.657259261213452e-22</v>
       </c>
       <c r="M15" t="n">
-        <v>-1.116608292726374e-17</v>
+        <v>4.663069666697254e-22</v>
       </c>
       <c r="N15" t="n">
-        <v>-1.123965446647801e-09</v>
+        <v>3.163231711937532e-22</v>
       </c>
       <c r="O15" t="n">
-        <v>-2.934005773875535e-17</v>
+        <v>4.986840889354011e-29</v>
       </c>
       <c r="P15" t="n">
-        <v>-1.123965076499193e-09</v>
+        <v>-2.009515843114686e-33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-1.052748482821025e-17</v>
+        <v>-3.972885375306269e-26</v>
       </c>
       <c r="B16" t="n">
-        <v>1.404956628631223e-09</v>
+        <v>5.834818475341819e-16</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.938248337995065e-17</v>
+        <v>-6.828561017748119e-11</v>
       </c>
       <c r="D16" t="n">
-        <v>-1.404956620864107e-09</v>
+        <v>6.82874156034956e-11</v>
       </c>
       <c r="E16" t="n">
-        <v>-3.11270299213541e-17</v>
+        <v>2.591562785905889e-15</v>
       </c>
       <c r="F16" t="n">
-        <v>3.158244630929679e-17</v>
+        <v>0.7071080691215335</v>
       </c>
       <c r="G16" t="n">
-        <v>2.649211528571618e-09</v>
+        <v>-0.707105493245123</v>
       </c>
       <c r="H16" t="n">
-        <v>-3.224405678397098e-22</v>
+        <v>-6.285102656045612e-26</v>
       </c>
       <c r="I16" t="n">
-        <v>-3.973817273417265e-09</v>
+        <v>1.72406981169169e-11</v>
       </c>
       <c r="J16" t="n">
-        <v>-4.214865313446378e-09</v>
+        <v>1.618371951295341e-11</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.999999999994696</v>
+        <v>-2.146038059803278e-11</v>
       </c>
       <c r="L16" t="n">
-        <v>-1.949441861296978e-15</v>
+        <v>1.509657307716026e-29</v>
       </c>
       <c r="M16" t="n">
-        <v>-4.21486659615155e-09</v>
+        <v>4.571615443381234e-22</v>
       </c>
       <c r="N16" t="n">
-        <v>-5.61982726673725e-09</v>
+        <v>5.921330619709791e-22</v>
       </c>
       <c r="O16" t="n">
-        <v>-1.130123477774968e-16</v>
+        <v>3.897903770349174e-22</v>
       </c>
       <c r="P16" t="n">
-        <v>-5.619825348997717e-09</v>
+        <v>-2.473721641472796e-33</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-2.649211528367556e-09</v>
+        <v>-1.243477728755538e-20</v>
       </c>
       <c r="B17" t="n">
-        <v>5.420165157900406e-16</v>
+        <v>6.438114179409845e-11</v>
       </c>
       <c r="C17" t="n">
-        <v>-2.809912515303486e-09</v>
+        <v>-6.828710217201182e-11</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.165145668180866e-16</v>
+        <v>-6.828592369026878e-11</v>
       </c>
       <c r="E17" t="n">
-        <v>-2.809913564369484e-09</v>
+        <v>-1.931434253822891e-10</v>
       </c>
       <c r="F17" t="n">
-        <v>2.616953862122222e-25</v>
+        <v>0.7071054932492159</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.052552982193521e-17</v>
+        <v>0.7071080691256262</v>
       </c>
       <c r="H17" t="n">
-        <v>1.302142065253608e-16</v>
+        <v>1.998447998379254e-21</v>
       </c>
       <c r="I17" t="n">
-        <v>-1</v>
+        <v>-1.800187511760553e-21</v>
       </c>
       <c r="J17" t="n">
-        <v>-2.809913210736469e-09</v>
+        <v>3.526542429072731e-22</v>
       </c>
       <c r="K17" t="n">
-        <v>3.973817329542457e-09</v>
+        <v>8.750411324752787e-22</v>
       </c>
       <c r="L17" t="n">
-        <v>-4.475940030048065e-16</v>
+        <v>-2.002119097619507e-32</v>
       </c>
       <c r="M17" t="n">
-        <v>2.809913230546428e-09</v>
+        <v>-1.637943704348285e-32</v>
       </c>
       <c r="N17" t="n">
-        <v>1.786573384063494e-17</v>
+        <v>-1.607478975179168e-32</v>
       </c>
       <c r="O17" t="n">
-        <v>1.090528666912025e-24</v>
+        <v>-1.313109907654873e-32</v>
       </c>
       <c r="P17" t="n">
-        <v>1.786572705712239e-17</v>
+        <v>5.088256987469149e-44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tries and other stufffffffff
</commit_message>
<xml_diff>
--- a/final_eigenvec_four.xlsx
+++ b/final_eigenvec_four.xlsx
@@ -517,49 +517,49 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1.036232854677933e-22</v>
+        <v>1.665374230732391e-22</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.681332379119761e-32</v>
+        <v>2.524364338824382e-32</v>
       </c>
       <c r="C2" t="n">
-        <v>-8.166549349893839e-23</v>
+        <v>1.352704871469615e-22</v>
       </c>
       <c r="D2" t="n">
-        <v>8.166690288005269e-23</v>
+        <v>-1.352749823090494e-22</v>
       </c>
       <c r="E2" t="n">
-        <v>3.111256778370345e-33</v>
+        <v>-2.760134611073494e-33</v>
       </c>
       <c r="F2" t="n">
-        <v>-4.617119692812142e-33</v>
+        <v>-5.128843399645042e-33</v>
       </c>
       <c r="G2" t="n">
-        <v>4.6171028718429e-33</v>
+        <v>5.128824909122333e-33</v>
       </c>
       <c r="H2" t="n">
-        <v>2.71564472260426e-22</v>
+        <v>4.344454514954092e-22</v>
       </c>
       <c r="I2" t="n">
-        <v>-4.658119932132633e-22</v>
+        <v>7.093829170853745e-22</v>
       </c>
       <c r="J2" t="n">
-        <v>8.042144018329229e-23</v>
+        <v>-4.992583390432867e-22</v>
       </c>
       <c r="K2" t="n">
-        <v>3.996898153757778e-22</v>
+        <v>7.199091411446751e-22</v>
       </c>
       <c r="L2" t="n">
-        <v>9.657171269114655e-12</v>
+        <v>-1.20714640863934e-11</v>
       </c>
       <c r="M2" t="n">
-        <v>1.016544344117341e-11</v>
+        <v>-1.287622835881957e-11</v>
       </c>
       <c r="N2" t="n">
-        <v>1.073019029901643e-11</v>
+        <v>-1.379595895587827e-11</v>
       </c>
       <c r="O2" t="n">
-        <v>1.136137796366431e-11</v>
+        <v>-1.48571865678687e-11</v>
       </c>
       <c r="P2" t="n">
         <v>1</v>
@@ -567,752 +567,752 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-1.07301896317416e-11</v>
+        <v>1.379595441334928e-11</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.93495569359993e-21</v>
+        <v>2.101680114068488e-21</v>
       </c>
       <c r="C3" t="n">
-        <v>7.066125231047504e-18</v>
+        <v>1.084597122394622e-17</v>
       </c>
       <c r="D3" t="n">
-        <v>-7.067056197319154e-18</v>
+        <v>-1.084389355574739e-17</v>
       </c>
       <c r="E3" t="n">
-        <v>4.002330981565128e-22</v>
+        <v>-1.423503335560283e-20</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.777411577244597e-22</v>
+        <v>1.143239369995058e-21</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.596100714375952e-22</v>
+        <v>-1.177489229829343e-21</v>
       </c>
       <c r="H3" t="n">
-        <v>2.146041825515863e-11</v>
+        <v>2.759190919626479e-11</v>
       </c>
       <c r="I3" t="n">
-        <v>-2.154232952819525e-11</v>
+        <v>1.273014087395436e-11</v>
       </c>
       <c r="J3" t="n">
-        <v>2.234731249473008e-11</v>
+        <v>-3.828693187204522e-11</v>
       </c>
       <c r="K3" t="n">
-        <v>1.631888509184236e-17</v>
+        <v>1.75902750105536e-17</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="M3" t="n">
-        <v>5.994110713235593e-15</v>
+        <v>3.366380189682996e-15</v>
       </c>
       <c r="N3" t="n">
-        <v>6.660187513674559e-16</v>
+        <v>-2.414850701961177e-15</v>
       </c>
       <c r="O3" t="n">
-        <v>-4.043647085677147e-16</v>
+        <v>3.249067041065305e-16</v>
       </c>
       <c r="P3" t="n">
-        <v>-9.656940896947432e-12</v>
+        <v>-1.207132318112019e-11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9.117503425189895e-18</v>
+        <v>6.569568230479623e-18</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.29335736330914e-23</v>
+        <v>6.428040652633421e-23</v>
       </c>
       <c r="C4" t="n">
-        <v>-7.187995025634125e-12</v>
+        <v>9.104715389730651e-12</v>
       </c>
       <c r="D4" t="n">
-        <v>7.188119076300633e-12</v>
+        <v>-9.105017948701963e-12</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.11106675629875e-21</v>
+        <v>7.105090464649326e-21</v>
       </c>
       <c r="F4" t="n">
-        <v>-8.729270386699821e-22</v>
+        <v>-1.627035819208651e-21</v>
       </c>
       <c r="G4" t="n">
-        <v>4.928775308882372e-22</v>
+        <v>1.555382260861803e-21</v>
       </c>
       <c r="H4" t="n">
-        <v>2.443626581453735e-17</v>
+        <v>-2.295471486847637e-17</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.50796173660397e-11</v>
+        <v>7.956372559978297e-12</v>
       </c>
       <c r="J4" t="n">
-        <v>1.564309955763869e-11</v>
+        <v>-2.392933034335652e-11</v>
       </c>
       <c r="K4" t="n">
-        <v>2.414294852692855e-11</v>
+        <v>3.219057925514334e-11</v>
       </c>
       <c r="L4" t="n">
-        <v>5.941540696923834e-17</v>
+        <v>-2.604846392911482e-16</v>
       </c>
       <c r="M4" t="n">
-        <v>6.106718605282241e-16</v>
+        <v>-9.782496747449399e-16</v>
       </c>
       <c r="N4" t="n">
-        <v>1.339266608542708e-15</v>
+        <v>-3.272359287040641e-15</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="P4" t="n">
-        <v>-1.136173316801328e-11</v>
+        <v>-1.485749474322401e-11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-1.110568744945022e-16</v>
+        <v>-1.375888438987634e-16</v>
       </c>
       <c r="B5" t="n">
-        <v>2.931721386475353e-17</v>
+        <v>1.960508313104706e-17</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.517449074881796e-11</v>
+        <v>1.951082183501514e-11</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.51748937261747e-11</v>
+        <v>1.951007645486497e-11</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.414323856242113e-11</v>
+        <v>3.219040585236756e-11</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.211193598966174e-16</v>
+        <v>8.305575431744415e-17</v>
       </c>
       <c r="G5" t="n">
-        <v>1.211050210022838e-16</v>
+        <v>-8.307143615362624e-17</v>
       </c>
       <c r="H5" t="n">
-        <v>2.195917947110037e-16</v>
+        <v>-2.650361544865463e-17</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.7807480474653604</v>
+        <v>0.3295527828388244</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8099215765986721</v>
+        <v>-0.9911558133533193</v>
       </c>
       <c r="K5" t="n">
-        <v>6.122626597949276e-17</v>
+        <v>5.409388983293431e-16</v>
       </c>
       <c r="L5" t="n">
-        <v>-2.759176053385392e-11</v>
+        <v>3.862860021013119e-11</v>
       </c>
       <c r="M5" t="n">
-        <v>-1.574023087392656e-16</v>
+        <v>7.016479167557147e-17</v>
       </c>
       <c r="N5" t="n">
-        <v>-8.995716286418389e-17</v>
+        <v>8.499726758271735e-17</v>
       </c>
       <c r="O5" t="n">
-        <v>-1.931424581946772e-11</v>
+        <v>2.414285421803879e-11</v>
       </c>
       <c r="P5" t="n">
-        <v>1.503558541149491e-22</v>
+        <v>2.476730230227017e-22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-9.657188836838101e-12</v>
+        <v>1.20714464047233e-11</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.756118195063036e-21</v>
+        <v>1.75793882695788e-21</v>
       </c>
       <c r="C6" t="n">
-        <v>1.319085049485686e-17</v>
+        <v>1.51460922534458e-17</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.319118218817301e-17</v>
+        <v>-1.514509750148364e-17</v>
       </c>
       <c r="E6" t="n">
-        <v>1.683647746509007e-21</v>
+        <v>-2.692349409069774e-20</v>
       </c>
       <c r="F6" t="n">
-        <v>7.799659062309739e-22</v>
+        <v>3.701622416185696e-21</v>
       </c>
       <c r="G6" t="n">
-        <v>-3.572209909903872e-22</v>
+        <v>-3.592567666980135e-21</v>
       </c>
       <c r="H6" t="n">
-        <v>-1.121540905332171e-17</v>
+        <v>3.719393792347411e-17</v>
       </c>
       <c r="I6" t="n">
-        <v>-1.34094410500141e-11</v>
+        <v>2.605052244088411e-11</v>
       </c>
       <c r="J6" t="n">
-        <v>-1.258732465393586e-11</v>
+        <v>3.661431873046316e-12</v>
       </c>
       <c r="K6" t="n">
-        <v>2.759189352235694e-11</v>
+        <v>3.862868595054531e-11</v>
       </c>
       <c r="L6" t="n">
-        <v>-6.213372908313923e-16</v>
+        <v>1.591012737683273e-15</v>
       </c>
       <c r="M6" t="n">
-        <v>-4.089820745680538e-15</v>
+        <v>2.207624148062156e-15</v>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O6" t="n">
-        <v>-3.056582764667324e-15</v>
+        <v>4.555383847910845e-15</v>
       </c>
       <c r="P6" t="n">
-        <v>-1.07286927637977e-11</v>
+        <v>-1.379419262672943e-11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.931434256379727e-10</v>
+        <v>1.931434288758194e-10</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.79145909033353e-16</v>
+        <v>9.97025833586315e-16</v>
       </c>
       <c r="D7" t="n">
-        <v>2.830006589978719e-16</v>
+        <v>-9.979222056809961e-16</v>
       </c>
       <c r="E7" t="n">
-        <v>6.43811430059132e-11</v>
+        <v>-6.438120148163163e-11</v>
       </c>
       <c r="F7" t="n">
-        <v>-1.51324093306471e-18</v>
+        <v>-2.757875719321384e-18</v>
       </c>
       <c r="G7" t="n">
-        <v>1.530787023740159e-18</v>
+        <v>2.775472420211469e-18</v>
       </c>
       <c r="H7" t="n">
-        <v>1.401137829263262e-16</v>
+        <v>4.701484335048023e-17</v>
       </c>
       <c r="I7" t="n">
-        <v>-2.554728460056816e-16</v>
+        <v>-1.150478492675772e-16</v>
       </c>
       <c r="J7" t="n">
-        <v>5.35963860758549e-17</v>
+        <v>7.026111492536771e-17</v>
       </c>
       <c r="K7" t="n">
-        <v>7.722582432092188e-17</v>
+        <v>-2.914335447595672e-16</v>
       </c>
       <c r="L7" t="n">
-        <v>-1.073019029903051e-11</v>
+        <v>1.379595895587471e-11</v>
       </c>
       <c r="M7" t="n">
-        <v>3.760756258047686e-23</v>
+        <v>1.037542581496375e-23</v>
       </c>
       <c r="N7" t="n">
-        <v>-9.6571712691485e-12</v>
+        <v>1.207146408638367e-11</v>
       </c>
       <c r="O7" t="n">
-        <v>1.022041877917098e-23</v>
+        <v>2.909823889434485e-24</v>
       </c>
       <c r="P7" t="n">
-        <v>1.036063555944485e-22</v>
+        <v>1.665141958277148e-22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.532980422344469e-16</v>
+        <v>-4.535232651725648e-16</v>
       </c>
       <c r="B8" t="n">
-        <v>-7.593513408075343e-19</v>
+        <v>9.541095414789774e-18</v>
       </c>
       <c r="C8" t="n">
-        <v>-9.151184712442485e-17</v>
+        <v>2.841197976332841e-16</v>
       </c>
       <c r="D8" t="n">
-        <v>9.327291057562296e-17</v>
+        <v>-2.912646725097674e-16</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.931440674250336e-11</v>
+        <v>2.414295406849748e-11</v>
       </c>
       <c r="F8" t="n">
-        <v>1.517480723843754e-11</v>
+        <v>1.951046635613485e-11</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.517475196535439e-11</v>
+        <v>-1.951039605059604e-11</v>
       </c>
       <c r="H8" t="n">
-        <v>-3.951529720224298e-17</v>
+        <v>1.095736445465087e-16</v>
       </c>
       <c r="I8" t="n">
-        <v>-1.085148659835906e-16</v>
+        <v>-3.888909814843483e-16</v>
       </c>
       <c r="J8" t="n">
-        <v>2.057559085583267e-16</v>
+        <v>2.012299220649949e-16</v>
       </c>
       <c r="K8" t="n">
         <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>-7.034652372932426e-19</v>
+        <v>-1.352587394875078e-24</v>
       </c>
       <c r="M8" t="n">
-        <v>4.285286258340713e-19</v>
+        <v>2.952979972853078e-24</v>
       </c>
       <c r="N8" t="n">
-        <v>-2.759191801217852e-11</v>
+        <v>3.862868507645693e-11</v>
       </c>
       <c r="O8" t="n">
-        <v>-2.414292816397255e-11</v>
+        <v>3.219057089704932e-11</v>
       </c>
       <c r="P8" t="n">
-        <v>1.706409072799458e-22</v>
+        <v>2.912136469209888e-22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-6.438079788469179e-11</v>
+        <v>6.438117675880091e-11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.541994180325995e-15</v>
+        <v>1.731020118964983e-17</v>
       </c>
       <c r="C9" t="n">
-        <v>-5.441272745586317e-16</v>
+        <v>5.557573719739602e-16</v>
       </c>
       <c r="D9" t="n">
-        <v>1.864211858351288e-15</v>
+        <v>9.367003398047486e-16</v>
       </c>
       <c r="E9" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.365703965208477e-10</v>
+        <v>-1.365724286741246e-10</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.365756551291545e-10</v>
+        <v>-1.365736229829842e-10</v>
       </c>
       <c r="H9" t="n">
-        <v>6.51289742165428e-17</v>
+        <v>-5.619536286739466e-17</v>
       </c>
       <c r="I9" t="n">
-        <v>1.884941967829163e-11</v>
+        <v>-1.060869609552739e-11</v>
       </c>
       <c r="J9" t="n">
-        <v>-1.955375358015932e-11</v>
+        <v>3.190581061690605e-11</v>
       </c>
       <c r="K9" t="n">
-        <v>-1.931427712973458e-11</v>
+        <v>-2.414300810704911e-11</v>
       </c>
       <c r="L9" t="n">
-        <v>4.933582038967252e-22</v>
+        <v>-9.206094933747034e-22</v>
       </c>
       <c r="M9" t="n">
-        <v>1.481658855806176e-25</v>
+        <v>2.234580334567129e-25</v>
       </c>
       <c r="N9" t="n">
-        <v>4.231201798904439e-22</v>
+        <v>-7.534202529190264e-22</v>
       </c>
       <c r="O9" t="n">
-        <v>4.663175341856139e-22</v>
+        <v>-7.771353461079868e-22</v>
       </c>
       <c r="P9" t="n">
-        <v>-2.342812185182386e-33</v>
+        <v>-5.04540302465266e-33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7.782943328115727e-18</v>
+        <v>1.565463539576653e-17</v>
       </c>
       <c r="B10" t="n">
-        <v>4.831206747893899e-22</v>
+        <v>-1.336428445804674e-22</v>
       </c>
       <c r="C10" t="n">
-        <v>-8.033655272116433e-12</v>
+        <v>1.050541947480566e-11</v>
       </c>
       <c r="D10" t="n">
-        <v>8.033793917072827e-12</v>
+        <v>-1.050576858222879e-11</v>
       </c>
       <c r="E10" t="n">
-        <v>-4.089991652730208e-22</v>
+        <v>3.366758073665463e-20</v>
       </c>
       <c r="F10" t="n">
-        <v>-5.420738390863429e-22</v>
+        <v>-3.908243614130491e-21</v>
       </c>
       <c r="G10" t="n">
-        <v>8.367266997640653e-22</v>
+        <v>3.905089793985532e-21</v>
       </c>
       <c r="H10" t="n">
-        <v>1.931429166024468e-11</v>
+        <v>2.414292264905585e-11</v>
       </c>
       <c r="I10" t="n">
-        <v>-1.508562958748424e-11</v>
+        <v>3.039238869299804e-11</v>
       </c>
       <c r="J10" t="n">
-        <v>-1.416077417627182e-11</v>
+        <v>4.271723893575094e-12</v>
       </c>
       <c r="K10" t="n">
-        <v>-1.228362757152175e-17</v>
+        <v>-2.682245524260773e-17</v>
       </c>
       <c r="L10" t="n">
-        <v>-5.513015296897995e-15</v>
+        <v>-2.672328160745508e-15</v>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="N10" t="n">
-        <v>5.567700535660178e-15</v>
+        <v>-1.945501226067442e-15</v>
       </c>
       <c r="O10" t="n">
-        <v>-1.198007077412873e-15</v>
+        <v>1.247757597534541e-15</v>
       </c>
       <c r="P10" t="n">
-        <v>-1.016482316582114e-11</v>
+        <v>-1.287568532257792e-11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7.422668723844378e-17</v>
+        <v>-1.90610959539296e-16</v>
       </c>
       <c r="B11" t="n">
-        <v>2.414292984068295e-11</v>
+        <v>-3.219056760967205e-11</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.951051822093606e-11</v>
+        <v>2.731489413278035e-11</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.951033888895094e-11</v>
+        <v>2.731431281809715e-11</v>
       </c>
       <c r="E11" t="n">
-        <v>7.132816766766335e-17</v>
+        <v>1.326357570909331e-16</v>
       </c>
       <c r="F11" t="n">
-        <v>-1.274664482070851e-18</v>
+        <v>-8.204792309764621e-18</v>
       </c>
       <c r="G11" t="n">
-        <v>1.266471142440308e-18</v>
+        <v>8.190220512194377e-18</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>8.586242091546045e-17</v>
+        <v>3.755887814602189e-16</v>
       </c>
       <c r="J11" t="n">
-        <v>7.927753658747034e-17</v>
+        <v>-4.105722334831291e-16</v>
       </c>
       <c r="K11" t="n">
-        <v>-1.47451497343439e-17</v>
+        <v>2.69540548887559e-16</v>
       </c>
       <c r="L11" t="n">
-        <v>-2.146024322006007e-11</v>
+        <v>2.759191791175844e-11</v>
       </c>
       <c r="M11" t="n">
-        <v>-1.931443291938531e-11</v>
+        <v>2.414292817278058e-11</v>
       </c>
       <c r="N11" t="n">
-        <v>2.24637446287797e-17</v>
+        <v>6.257280680690587e-24</v>
       </c>
       <c r="O11" t="n">
-        <v>-2.065563270140633e-18</v>
+        <v>-2.104002919209558e-24</v>
       </c>
       <c r="P11" t="n">
-        <v>1.320040313855912e-22</v>
+        <v>2.094822528617904e-22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.600739220577689e-16</v>
+        <v>-1.262149164225921e-15</v>
       </c>
       <c r="B12" t="n">
-        <v>-2.522237112090684e-15</v>
+        <v>1.154200975251423e-15</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.7071006793750427</v>
+        <v>0.7070950659087049</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7071128825524579</v>
+        <v>-0.7071185633971495</v>
       </c>
       <c r="E12" t="n">
-        <v>7.044424980886948e-17</v>
+        <v>3.204114339881421e-16</v>
       </c>
       <c r="F12" t="n">
-        <v>-6.828663451425932e-11</v>
+        <v>-6.828662951612312e-11</v>
       </c>
       <c r="G12" t="n">
-        <v>6.828638575721117e-11</v>
+        <v>6.828638341608807e-11</v>
       </c>
       <c r="H12" t="n">
-        <v>-4.906190289695546e-16</v>
+        <v>2.344009897043123e-16</v>
       </c>
       <c r="I12" t="n">
-        <v>-2.300957280430481e-16</v>
+        <v>9.469222565548587e-17</v>
       </c>
       <c r="J12" t="n">
-        <v>3.488532565669355e-17</v>
+        <v>1.190172222066886e-17</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.937106113283201e-17</v>
+        <v>2.042358407885334e-16</v>
       </c>
       <c r="L12" t="n">
-        <v>2.106310406990328e-24</v>
+        <v>1.231769214506349e-24</v>
       </c>
       <c r="M12" t="n">
-        <v>-1.136137796367196e-11</v>
+        <v>1.485718656786489e-11</v>
       </c>
       <c r="N12" t="n">
-        <v>8.442281831172406e-24</v>
+        <v>4.340275290830633e-24</v>
       </c>
       <c r="O12" t="n">
-        <v>-1.016544344117642e-11</v>
+        <v>1.287622835881807e-11</v>
       </c>
       <c r="P12" t="n">
-        <v>1.154900087443605e-22</v>
+        <v>1.913004272763913e-22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-2.004483291426057e-25</v>
+        <v>-2.326062693822745e-25</v>
       </c>
       <c r="B13" t="n">
-        <v>4.734144518475036e-15</v>
+        <v>-1.241579225390183e-15</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.7071128829453985</v>
+        <v>0.7071184962702959</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.7071006797679902</v>
+        <v>0.7070949987796202</v>
       </c>
       <c r="E13" t="n">
-        <v>-1.923134077490348e-16</v>
+        <v>-6.808451113457802e-16</v>
       </c>
       <c r="F13" t="n">
-        <v>-6.828645794206624e-11</v>
+        <v>-6.828660696150925e-11</v>
       </c>
       <c r="G13" t="n">
-        <v>-6.828656788795495e-11</v>
+        <v>-6.828641886836668e-11</v>
       </c>
       <c r="H13" t="n">
-        <v>-2.759191791175646e-11</v>
+        <v>-3.862868507645601e-11</v>
       </c>
       <c r="I13" t="n">
-        <v>1.675503192581534e-11</v>
+        <v>-9.092966050562929e-12</v>
       </c>
       <c r="J13" t="n">
-        <v>-1.738122816398455e-11</v>
+        <v>2.734787184700931e-11</v>
       </c>
       <c r="K13" t="n">
-        <v>-2.182431025882176e-25</v>
+        <v>-8.715238596914975e-26</v>
       </c>
       <c r="L13" t="n">
-        <v>5.921275742077835e-22</v>
+        <v>-1.065837667222179e-21</v>
       </c>
       <c r="M13" t="n">
-        <v>3.485224005666194e-22</v>
+        <v>-5.794339357851038e-22</v>
       </c>
       <c r="N13" t="n">
-        <v>4.35120607344181e-28</v>
+        <v>-6.981834875761937e-28</v>
       </c>
       <c r="O13" t="n">
-        <v>2.996742145423013e-22</v>
+        <v>-4.766661924972722e-22</v>
       </c>
       <c r="P13" t="n">
-        <v>-2.13436292205868e-33</v>
+        <v>-4.472847828317725e-33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6.37286102559884e-17</v>
+        <v>-1.5756342512065e-16</v>
       </c>
       <c r="B14" t="n">
-        <v>1.931421085411896e-11</v>
+        <v>-2.414290007734553e-11</v>
       </c>
       <c r="C14" t="n">
-        <v>3.562859036743195e-16</v>
+        <v>-8.041775851746166e-17</v>
       </c>
       <c r="D14" t="n">
-        <v>1.720734678578681e-17</v>
+        <v>7.878977529051663e-17</v>
       </c>
       <c r="E14" t="n">
-        <v>-1.705925861010295e-16</v>
+        <v>-1.038105732383381e-17</v>
       </c>
       <c r="F14" t="n">
-        <v>1.951046815470161e-11</v>
+        <v>2.731455399390334e-11</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.951039708355994e-11</v>
+        <v>-2.731445555949354e-11</v>
       </c>
       <c r="H14" t="n">
-        <v>1.544619257860951e-16</v>
+        <v>-7.29157315092532e-18</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.6248459701230595</v>
+        <v>0.944137152813714</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.5865381826956547</v>
+        <v>0.1327032541270937</v>
       </c>
       <c r="K14" t="n">
-        <v>1.672549891932644e-16</v>
+        <v>2.209214383758155e-16</v>
       </c>
       <c r="L14" t="n">
-        <v>-8.869756629800233e-25</v>
+        <v>-1.09590350685046e-25</v>
       </c>
       <c r="M14" t="n">
-        <v>-2.414292817278483e-11</v>
+        <v>3.219057089704948e-11</v>
       </c>
       <c r="N14" t="n">
-        <v>-2.14603805980339e-11</v>
+        <v>2.759191791175612e-11</v>
       </c>
       <c r="O14" t="n">
-        <v>2.579890704434267e-25</v>
+        <v>-1.675666780433509e-25</v>
       </c>
       <c r="P14" t="n">
-        <v>1.49428971361494e-22</v>
+        <v>2.452460505825282e-22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-1.931434253822939e-10</v>
+        <v>1.931434253822951e-10</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C15" t="n">
-        <v>9.226093206815878e-16</v>
+        <v>-5.797682360548315e-16</v>
       </c>
       <c r="D15" t="n">
-        <v>4.078367769298119e-15</v>
+        <v>-2.271909548600767e-15</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.12611528290278e-15</v>
+        <v>1.457283827394942e-17</v>
       </c>
       <c r="F15" t="n">
-        <v>-4.552476976591992e-11</v>
+        <v>-4.55242756308276e-11</v>
       </c>
       <c r="G15" t="n">
-        <v>-4.552391412263053e-11</v>
+        <v>-4.552440825531886e-11</v>
       </c>
       <c r="H15" t="n">
-        <v>-2.414292817278628e-11</v>
+        <v>-3.219057089706281e-11</v>
       </c>
       <c r="I15" t="n">
-        <v>1.206842813504288e-11</v>
+        <v>-2.279430734335372e-11</v>
       </c>
       <c r="J15" t="n">
-        <v>1.132854215111745e-11</v>
+        <v>-3.203745108759551e-12</v>
       </c>
       <c r="K15" t="n">
-        <v>2.844064444401423e-25</v>
+        <v>3.328109496085297e-25</v>
       </c>
       <c r="L15" t="n">
-        <v>3.657259261213452e-22</v>
+        <v>-6.149074082706975e-22</v>
       </c>
       <c r="M15" t="n">
-        <v>4.663069666697254e-22</v>
+        <v>-7.77174641007935e-22</v>
       </c>
       <c r="N15" t="n">
-        <v>3.163231711937532e-22</v>
+        <v>-5.107147640916535e-22</v>
       </c>
       <c r="O15" t="n">
-        <v>4.986840889354011e-29</v>
+        <v>9.948612767191988e-35</v>
       </c>
       <c r="P15" t="n">
-        <v>-2.009515843114686e-33</v>
+        <v>-4.13683959236623e-33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-3.972885375306269e-26</v>
+        <v>-9.110429739083297e-26</v>
       </c>
       <c r="B16" t="n">
-        <v>5.834818475341819e-16</v>
+        <v>1.589774002716592e-16</v>
       </c>
       <c r="C16" t="n">
-        <v>-6.828561017748119e-11</v>
+        <v>6.828548122608369e-11</v>
       </c>
       <c r="D16" t="n">
-        <v>6.82874156034956e-11</v>
+        <v>-6.828755107045754e-11</v>
       </c>
       <c r="E16" t="n">
-        <v>2.591562785905889e-15</v>
+        <v>1.126734025035226e-16</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7071080691215335</v>
+        <v>0.70710805536802</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.707105493245123</v>
+        <v>-0.7071055070027789</v>
       </c>
       <c r="H16" t="n">
-        <v>-6.285102656045612e-26</v>
+        <v>3.743438718584211e-26</v>
       </c>
       <c r="I16" t="n">
-        <v>1.72406981169169e-11</v>
+        <v>-3.647085296111135e-11</v>
       </c>
       <c r="J16" t="n">
-        <v>1.618371951295341e-11</v>
+        <v>-5.126282407211175e-12</v>
       </c>
       <c r="K16" t="n">
-        <v>-2.146038059803278e-11</v>
+        <v>-2.759191791175633e-11</v>
       </c>
       <c r="L16" t="n">
-        <v>1.509657307716026e-29</v>
+        <v>3.431099875263232e-34</v>
       </c>
       <c r="M16" t="n">
-        <v>4.571615443381234e-22</v>
+        <v>-8.260877303035707e-22</v>
       </c>
       <c r="N16" t="n">
-        <v>5.921330619709791e-22</v>
+        <v>-1.065839507667986e-21</v>
       </c>
       <c r="O16" t="n">
-        <v>3.897903770349174e-22</v>
+        <v>-6.695658445613472e-22</v>
       </c>
       <c r="P16" t="n">
-        <v>-2.473721641472796e-33</v>
+        <v>-5.4050651607276e-33</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-1.243477728755538e-20</v>
+        <v>1.243479557629784e-20</v>
       </c>
       <c r="B17" t="n">
-        <v>6.438114179409845e-11</v>
+        <v>-6.438114179409828e-11</v>
       </c>
       <c r="C17" t="n">
-        <v>-6.828710217201182e-11</v>
+        <v>6.828764426041128e-11</v>
       </c>
       <c r="D17" t="n">
-        <v>-6.828592369026878e-11</v>
+        <v>6.828537506749272e-11</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.931434253822891e-10</v>
+        <v>1.93143425382295e-10</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7071054932492159</v>
+        <v>0.707105507002779</v>
       </c>
       <c r="G17" t="n">
-        <v>0.7071080691256262</v>
+        <v>0.7071080553680201</v>
       </c>
       <c r="H17" t="n">
-        <v>1.998447998379254e-21</v>
+        <v>4.559432667379332e-21</v>
       </c>
       <c r="I17" t="n">
-        <v>-1.800187511760553e-21</v>
+        <v>2.897928656279906e-21</v>
       </c>
       <c r="J17" t="n">
-        <v>3.526542429072731e-22</v>
+        <v>-2.227570613316149e-21</v>
       </c>
       <c r="K17" t="n">
-        <v>8.750411324752787e-22</v>
+        <v>1.42746543255417e-21</v>
       </c>
       <c r="L17" t="n">
-        <v>-2.002119097619507e-32</v>
+        <v>5.024271810181825e-32</v>
       </c>
       <c r="M17" t="n">
-        <v>-1.637943704348285e-32</v>
+        <v>3.832215787878858e-32</v>
       </c>
       <c r="N17" t="n">
-        <v>-1.607478975179168e-32</v>
+        <v>3.750088912921917e-32</v>
       </c>
       <c r="O17" t="n">
-        <v>-1.313109907654873e-32</v>
+        <v>2.857597990731825e-32</v>
       </c>
       <c r="P17" t="n">
-        <v>5.088256987469149e-44</v>
+        <v>1.415430784746575e-43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pegasus and non degenerate spectrum for 4 qubits
</commit_message>
<xml_diff>
--- a/final_eigenvec_four.xlsx
+++ b/final_eigenvec_four.xlsx
@@ -517,802 +517,802 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.665374230732391e-22</v>
+        <v>2.231748711887562e-38</v>
       </c>
       <c r="B2" t="n">
-        <v>2.524364338824382e-32</v>
+        <v>-1</v>
       </c>
       <c r="C2" t="n">
-        <v>1.352704871469615e-22</v>
+        <v>-7.742867047255508e-33</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.352749823090494e-22</v>
+        <v>-8.778053409629295e-33</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.760134611073494e-33</v>
+        <v>1.000711151416789e-32</v>
       </c>
       <c r="F2" t="n">
-        <v>-5.128843399645042e-33</v>
+        <v>-1.063809148423803e-32</v>
       </c>
       <c r="G2" t="n">
-        <v>5.128824909122333e-33</v>
+        <v>-5.680688981832213e-12</v>
       </c>
       <c r="H2" t="n">
-        <v>4.344454514954092e-22</v>
+        <v>5.365095149508155e-12</v>
       </c>
       <c r="I2" t="n">
-        <v>7.093829170853745e-22</v>
+        <v>5.082721720586695e-12</v>
       </c>
       <c r="J2" t="n">
-        <v>-4.992583390432867e-22</v>
+        <v>4.828585634557375e-12</v>
       </c>
       <c r="K2" t="n">
-        <v>7.199091411446751e-22</v>
+        <v>2.590589034758215e-22</v>
       </c>
       <c r="L2" t="n">
-        <v>-1.20714640863934e-11</v>
+        <v>-2.260871682934731e-22</v>
       </c>
       <c r="M2" t="n">
-        <v>-1.287622835881957e-11</v>
+        <v>-2.727604027577546e-22</v>
       </c>
       <c r="N2" t="n">
-        <v>-1.379595895587827e-11</v>
+        <v>1.816409443589286e-22</v>
       </c>
       <c r="O2" t="n">
-        <v>-1.48571865678687e-11</v>
+        <v>1.619113835452105e-22</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>-1.367827367468036e-22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.379595441334928e-11</v>
+        <v>-1.676570567569614e-27</v>
       </c>
       <c r="B3" t="n">
-        <v>2.101680114068488e-21</v>
+        <v>-5.680668107585969e-12</v>
       </c>
       <c r="C3" t="n">
-        <v>1.084597122394622e-17</v>
+        <v>3.85655271134106e-22</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.084389355574739e-17</v>
+        <v>5.240338119386222e-22</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.423503335560283e-20</v>
+        <v>-7.347910382971129e-22</v>
       </c>
       <c r="F3" t="n">
-        <v>1.143239369995058e-21</v>
+        <v>4.205674416784645e-25</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.177489229829343e-21</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>2.759190919626479e-11</v>
+        <v>1.59373753636074e-15</v>
       </c>
       <c r="I3" t="n">
-        <v>1.273014087395436e-11</v>
+        <v>3.463733789554758e-16</v>
       </c>
       <c r="J3" t="n">
-        <v>-3.828693187204522e-11</v>
+        <v>-2.685260349080509e-17</v>
       </c>
       <c r="K3" t="n">
-        <v>1.75902750105536e-17</v>
+        <v>-2.414288686539947e-11</v>
       </c>
       <c r="L3" t="n">
-        <v>-1</v>
+        <v>1.931436229006388e-11</v>
       </c>
       <c r="M3" t="n">
-        <v>3.366380189682996e-15</v>
+        <v>1.196348392284316e-11</v>
       </c>
       <c r="N3" t="n">
-        <v>-2.414850701961177e-15</v>
+        <v>-1.599932499007658e-11</v>
       </c>
       <c r="O3" t="n">
-        <v>3.249067041065305e-16</v>
+        <v>-3.735920532742194e-17</v>
       </c>
       <c r="P3" t="n">
-        <v>-1.207132318112019e-11</v>
+        <v>-5.238184556469196e-18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6.569568230479623e-18</v>
+        <v>8.23783031182093e-28</v>
       </c>
       <c r="B4" t="n">
-        <v>6.428040652633421e-23</v>
+        <v>-5.364996991355424e-12</v>
       </c>
       <c r="C4" t="n">
-        <v>9.104715389730651e-12</v>
+        <v>2.995545540357545e-22</v>
       </c>
       <c r="D4" t="n">
-        <v>-9.105017948701963e-12</v>
+        <v>3.934106318070613e-22</v>
       </c>
       <c r="E4" t="n">
-        <v>7.105090464649326e-21</v>
+        <v>4.083130655631688e-24</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.627035819208651e-21</v>
+        <v>7.328767689235939e-22</v>
       </c>
       <c r="G4" t="n">
-        <v>1.555382260861803e-21</v>
+        <v>2.244109629531476e-15</v>
       </c>
       <c r="H4" t="n">
-        <v>-2.295471486847637e-17</v>
+        <v>-1</v>
       </c>
       <c r="I4" t="n">
-        <v>7.956372559978297e-12</v>
+        <v>-2.888508131220564e-15</v>
       </c>
       <c r="J4" t="n">
-        <v>-2.392933034335652e-11</v>
+        <v>1.162482032676207e-16</v>
       </c>
       <c r="K4" t="n">
-        <v>3.219057925514334e-11</v>
+        <v>-3.219086070912584e-11</v>
       </c>
       <c r="L4" t="n">
-        <v>-2.604846392911482e-16</v>
+        <v>-3.8791428784834e-17</v>
       </c>
       <c r="M4" t="n">
-        <v>-9.782496747449399e-16</v>
+        <v>1.292066551498168e-11</v>
       </c>
       <c r="N4" t="n">
-        <v>-3.272359287040641e-15</v>
+        <v>2.10554705060834e-12</v>
       </c>
       <c r="O4" t="n">
-        <v>-1</v>
+        <v>-1.609525049005667e-11</v>
       </c>
       <c r="P4" t="n">
-        <v>-1.485749474322401e-11</v>
+        <v>4.189814855976344e-18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-1.375888438987634e-16</v>
+        <v>-3.364924551939469e-20</v>
       </c>
       <c r="B5" t="n">
-        <v>1.960508313104706e-17</v>
+        <v>-5.080092504873385e-23</v>
       </c>
       <c r="C5" t="n">
-        <v>1.951082183501514e-11</v>
+        <v>1.073022212612199e-11</v>
       </c>
       <c r="D5" t="n">
-        <v>1.951007645486497e-11</v>
+        <v>1.207146284773652e-11</v>
       </c>
       <c r="E5" t="n">
-        <v>3.219040585236756e-11</v>
+        <v>7.922436495644798e-18</v>
       </c>
       <c r="F5" t="n">
-        <v>8.305575431744415e-17</v>
+        <v>-2.096557156088592e-18</v>
       </c>
       <c r="G5" t="n">
-        <v>-8.307143615362624e-17</v>
+        <v>2.414293677282866e-11</v>
       </c>
       <c r="H5" t="n">
-        <v>-2.650361544865463e-17</v>
+        <v>-3.219053908875856e-11</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3295527828388244</v>
+        <v>-6.935492123487756e-17</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.9911558133533193</v>
+        <v>7.768514086828277e-17</v>
       </c>
       <c r="K5" t="n">
-        <v>5.409388983293431e-16</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>3.862860021013119e-11</v>
+        <v>-9.482450287234275e-16</v>
       </c>
       <c r="M5" t="n">
-        <v>7.016479167557147e-17</v>
+        <v>-5.115920704346041e-16</v>
       </c>
       <c r="N5" t="n">
-        <v>8.499726758271735e-17</v>
+        <v>1.878791722238532e-16</v>
       </c>
       <c r="O5" t="n">
-        <v>2.414285421803879e-11</v>
+        <v>7.193873508046173e-16</v>
       </c>
       <c r="P5" t="n">
-        <v>2.476730230227017e-22</v>
+        <v>5.848981445822339e-17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.20714464047233e-11</v>
+        <v>-4.99885168993216e-28</v>
       </c>
       <c r="B6" t="n">
-        <v>1.75793882695788e-21</v>
+        <v>-5.082506165490012e-12</v>
       </c>
       <c r="C6" t="n">
-        <v>1.51460922534458e-17</v>
+        <v>3.075915050389118e-22</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.514509750148364e-17</v>
+        <v>2.028460970955706e-23</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.692349409069774e-20</v>
+        <v>-4.085231648467161e-22</v>
       </c>
       <c r="F6" t="n">
-        <v>3.701622416185696e-21</v>
+        <v>5.255744452222151e-22</v>
       </c>
       <c r="G6" t="n">
-        <v>-3.592567666980135e-21</v>
+        <v>8.322573545403726e-16</v>
       </c>
       <c r="H6" t="n">
-        <v>3.719393792347411e-17</v>
+        <v>2.32184985901952e-15</v>
       </c>
       <c r="I6" t="n">
-        <v>2.605052244088411e-11</v>
+        <v>-1</v>
       </c>
       <c r="J6" t="n">
-        <v>3.661431873046316e-12</v>
+        <v>-3.091246208778218e-15</v>
       </c>
       <c r="K6" t="n">
-        <v>3.862868595054531e-11</v>
+        <v>6.057036818255381e-16</v>
       </c>
       <c r="L6" t="n">
-        <v>1.591012737683273e-15</v>
+        <v>3.219058922451045e-11</v>
       </c>
       <c r="M6" t="n">
-        <v>2.207624148062156e-15</v>
+        <v>1.615080698047608e-11</v>
       </c>
       <c r="N6" t="n">
-        <v>-1</v>
+        <v>2.631950403890046e-12</v>
       </c>
       <c r="O6" t="n">
-        <v>4.555383847910845e-15</v>
+        <v>4.215569406829698e-17</v>
       </c>
       <c r="P6" t="n">
-        <v>-1.379419262672943e-11</v>
+        <v>1.60952930576039e-11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>-1.007155139870415e-22</v>
       </c>
       <c r="B7" t="n">
-        <v>1.931434288758194e-10</v>
+        <v>-4.724130262788954e-23</v>
       </c>
       <c r="C7" t="n">
-        <v>9.97025833586315e-16</v>
+        <v>9.657229951783325e-12</v>
       </c>
       <c r="D7" t="n">
-        <v>-9.979222056809961e-16</v>
+        <v>-1.848531944548585e-17</v>
       </c>
       <c r="E7" t="n">
-        <v>-6.438120148163163e-11</v>
+        <v>-1.207143380096243e-11</v>
       </c>
       <c r="F7" t="n">
-        <v>-2.757875719321384e-18</v>
+        <v>-9.549798273697313e-18</v>
       </c>
       <c r="G7" t="n">
-        <v>2.775472420211469e-18</v>
+        <v>1.931434253825439e-11</v>
       </c>
       <c r="H7" t="n">
-        <v>4.701484335048023e-17</v>
+        <v>3.410345917924417e-24</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.150478492675772e-16</v>
+        <v>-3.219057089704619e-11</v>
       </c>
       <c r="J7" t="n">
-        <v>7.026111492536771e-17</v>
+        <v>-2.452461525403291e-24</v>
       </c>
       <c r="K7" t="n">
-        <v>-2.914335447595672e-16</v>
+        <v>-1.259370550597011e-15</v>
       </c>
       <c r="L7" t="n">
-        <v>1.379595895587471e-11</v>
+        <v>-1</v>
       </c>
       <c r="M7" t="n">
-        <v>1.037542581496375e-23</v>
+        <v>9.636289446242676e-16</v>
       </c>
       <c r="N7" t="n">
-        <v>1.207146408638367e-11</v>
+        <v>-5.534092425119255e-16</v>
       </c>
       <c r="O7" t="n">
-        <v>2.909823889434485e-24</v>
+        <v>1.053792632085691e-15</v>
       </c>
       <c r="P7" t="n">
-        <v>1.665141958277148e-22</v>
+        <v>3.391134320120824e-16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-4.535232651725648e-16</v>
+        <v>3.093488856205732e-17</v>
       </c>
       <c r="B8" t="n">
-        <v>9.541095414789774e-18</v>
+        <v>-4.386088127070814e-23</v>
       </c>
       <c r="C8" t="n">
-        <v>2.841197976332841e-16</v>
+        <v>8.779164453220413e-12</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.912646725097674e-16</v>
+        <v>7.327766258857363e-17</v>
       </c>
       <c r="E8" t="n">
-        <v>2.414295406849748e-11</v>
+        <v>1.432019698021412e-16</v>
       </c>
       <c r="F8" t="n">
-        <v>1.951046635613485e-11</v>
+        <v>1.207131452158868e-11</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.951039605059604e-11</v>
+        <v>8.826464305920726e-26</v>
       </c>
       <c r="H8" t="n">
-        <v>1.095736445465087e-16</v>
+        <v>-1.931434253822927e-11</v>
       </c>
       <c r="I8" t="n">
-        <v>-3.888909814843483e-16</v>
+        <v>-2.414292817278689e-11</v>
       </c>
       <c r="J8" t="n">
-        <v>2.012299220649949e-16</v>
+        <v>1.034453723025051e-25</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>-1.109909007560883e-15</v>
       </c>
       <c r="L8" t="n">
-        <v>-1.352587394875078e-24</v>
+        <v>-1.516375350366841e-15</v>
       </c>
       <c r="M8" t="n">
-        <v>2.952979972853078e-24</v>
+        <v>-0.6689647316216069</v>
       </c>
       <c r="N8" t="n">
-        <v>3.862868507645693e-11</v>
+        <v>-0.1090164664112791</v>
       </c>
       <c r="O8" t="n">
-        <v>3.219057089704932e-11</v>
+        <v>-5.0146187834951e-17</v>
       </c>
       <c r="P8" t="n">
-        <v>2.912136469209888e-22</v>
+        <v>5.800604126749346e-16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6.438117675880091e-11</v>
+        <v>4.389624060269413e-12</v>
       </c>
       <c r="B9" t="n">
-        <v>1.731020118964983e-17</v>
+        <v>-1.141901946943713e-33</v>
       </c>
       <c r="C9" t="n">
-        <v>5.557573719739602e-16</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>9.367003398047486e-16</v>
+        <v>-1.397033491803106e-15</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>1.070798920892243e-16</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.365724286741246e-10</v>
+        <v>-1.452738233480887e-17</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.365736229829842e-10</v>
+        <v>-8.39351447153323e-22</v>
       </c>
       <c r="H9" t="n">
-        <v>-5.619536286739466e-17</v>
+        <v>8.289799725241271e-22</v>
       </c>
       <c r="I9" t="n">
-        <v>-1.060869609552739e-11</v>
+        <v>7.771777564969107e-22</v>
       </c>
       <c r="J9" t="n">
-        <v>3.190581061690605e-11</v>
+        <v>3.226394493872073e-27</v>
       </c>
       <c r="K9" t="n">
-        <v>-2.414300810704911e-11</v>
+        <v>-1.073024865693331e-11</v>
       </c>
       <c r="L9" t="n">
-        <v>-9.206094933747034e-22</v>
+        <v>9.657193530485186e-12</v>
       </c>
       <c r="M9" t="n">
-        <v>2.234580334567129e-25</v>
+        <v>5.873286546139251e-12</v>
       </c>
       <c r="N9" t="n">
-        <v>-7.534202529190264e-22</v>
+        <v>9.569053443397464e-13</v>
       </c>
       <c r="O9" t="n">
-        <v>-7.771353461079868e-22</v>
+        <v>3.478292783793902e-18</v>
       </c>
       <c r="P9" t="n">
-        <v>-5.04540302465266e-33</v>
+        <v>6.138332075495001e-18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.565463539576653e-17</v>
+        <v>-2.709834350789274e-27</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.336428445804674e-22</v>
+        <v>-4.828325407330431e-12</v>
       </c>
       <c r="C10" t="n">
-        <v>1.050541947480566e-11</v>
+        <v>-3.067266319856915e-23</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.050576858222879e-11</v>
+        <v>2.439254143947731e-22</v>
       </c>
       <c r="E10" t="n">
-        <v>3.366758073665463e-20</v>
+        <v>-3.114995750692445e-22</v>
       </c>
       <c r="F10" t="n">
-        <v>-3.908243614130491e-21</v>
+        <v>3.934873833296838e-22</v>
       </c>
       <c r="G10" t="n">
-        <v>3.905089793985532e-21</v>
+        <v>3.689603067076522e-16</v>
       </c>
       <c r="H10" t="n">
-        <v>2.414292264905585e-11</v>
+        <v>-2.482392588656102e-16</v>
       </c>
       <c r="I10" t="n">
-        <v>3.039238869299804e-11</v>
+        <v>2.638685493388011e-15</v>
       </c>
       <c r="J10" t="n">
-        <v>4.271723893575094e-12</v>
+        <v>-1</v>
       </c>
       <c r="K10" t="n">
-        <v>-2.682245524260773e-17</v>
+        <v>-5.072008259540997e-16</v>
       </c>
       <c r="L10" t="n">
-        <v>-2.672328160745508e-15</v>
+        <v>7.121684356580467e-19</v>
       </c>
       <c r="M10" t="n">
-        <v>-1</v>
+        <v>2.39270193881347e-11</v>
       </c>
       <c r="N10" t="n">
-        <v>-1.945501226067442e-15</v>
+        <v>-3.199868430412053e-11</v>
       </c>
       <c r="O10" t="n">
-        <v>1.247757597534541e-15</v>
+        <v>-2.414296792954197e-11</v>
       </c>
       <c r="P10" t="n">
-        <v>-1.287568532257792e-11</v>
+        <v>1.931433613125746e-11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-1.90610959539296e-16</v>
+        <v>3.990565576023635e-17</v>
       </c>
       <c r="B11" t="n">
-        <v>-3.219056760967205e-11</v>
+        <v>-4.411731537076132e-23</v>
       </c>
       <c r="C11" t="n">
-        <v>2.731489413278035e-11</v>
+        <v>-6.275049293301945e-17</v>
       </c>
       <c r="D11" t="n">
-        <v>2.731431281809715e-11</v>
+        <v>9.657073033623012e-12</v>
       </c>
       <c r="E11" t="n">
-        <v>1.326357570909331e-16</v>
+        <v>-1.073019920959177e-11</v>
       </c>
       <c r="F11" t="n">
-        <v>-8.204792309764621e-18</v>
+        <v>-7.515099769079732e-17</v>
       </c>
       <c r="G11" t="n">
-        <v>8.190220512194377e-18</v>
+        <v>1.609528544852462e-11</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>-1.030582811001717e-26</v>
       </c>
       <c r="I11" t="n">
-        <v>3.755887814602189e-16</v>
+        <v>5.666405316807146e-25</v>
       </c>
       <c r="J11" t="n">
-        <v>-4.105722334831291e-16</v>
+        <v>-3.219057089704946e-11</v>
       </c>
       <c r="K11" t="n">
-        <v>2.69540548887559e-16</v>
+        <v>1.674625396984456e-16</v>
       </c>
       <c r="L11" t="n">
-        <v>2.759191791175844e-11</v>
+        <v>-2.761973912883562e-17</v>
       </c>
       <c r="M11" t="n">
-        <v>2.414292817278058e-11</v>
+        <v>-0.7432941462479248</v>
       </c>
       <c r="N11" t="n">
-        <v>6.257280680690587e-24</v>
+        <v>0.9940399438911891</v>
       </c>
       <c r="O11" t="n">
-        <v>-2.104002919209558e-24</v>
+        <v>-6.405068774807477e-16</v>
       </c>
       <c r="P11" t="n">
-        <v>2.094822528617904e-22</v>
+        <v>5.814498672251493e-16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-1.262149164225921e-15</v>
+        <v>2.318992847370914e-20</v>
       </c>
       <c r="B12" t="n">
-        <v>1.154200975251423e-15</v>
+        <v>-4.101484788679566e-23</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7070950659087049</v>
+        <v>-6.26126423518508e-17</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.7071185633971495</v>
+        <v>8.779264969891236e-12</v>
       </c>
       <c r="E12" t="n">
-        <v>3.204114339881421e-16</v>
+        <v>-2.996622578430979e-17</v>
       </c>
       <c r="F12" t="n">
-        <v>-6.828662951612312e-11</v>
+        <v>1.073019912382238e-11</v>
       </c>
       <c r="G12" t="n">
-        <v>6.828638341608807e-11</v>
+        <v>-4.300665460244105e-22</v>
       </c>
       <c r="H12" t="n">
-        <v>2.344009897043123e-16</v>
+        <v>-1.609528544858974e-11</v>
       </c>
       <c r="I12" t="n">
-        <v>9.469222565548587e-17</v>
+        <v>1.396007887053938e-23</v>
       </c>
       <c r="J12" t="n">
-        <v>1.190172222066886e-17</v>
+        <v>-2.414292817279615e-11</v>
       </c>
       <c r="K12" t="n">
-        <v>2.042358407885334e-16</v>
+        <v>-6.810427651453845e-16</v>
       </c>
       <c r="L12" t="n">
-        <v>1.231769214506349e-24</v>
+        <v>8.867588615505553e-16</v>
       </c>
       <c r="M12" t="n">
-        <v>1.485718656786489e-11</v>
+        <v>-3.26704854165604e-16</v>
       </c>
       <c r="N12" t="n">
-        <v>4.340275290830633e-24</v>
+        <v>5.905304717420313e-16</v>
       </c>
       <c r="O12" t="n">
-        <v>1.287622835881807e-11</v>
+        <v>1</v>
       </c>
       <c r="P12" t="n">
-        <v>1.913004272763913e-22</v>
+        <v>2.012757527758671e-15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-2.326062693822745e-25</v>
+        <v>4.198762716307365e-12</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.241579225390183e-15</v>
+        <v>-1.009985749897254e-33</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7071184962702959</v>
+        <v>9.636416885034894e-16</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7070949987796202</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>-6.808451113457802e-16</v>
+        <v>-5.36500094496427e-17</v>
       </c>
       <c r="F13" t="n">
-        <v>-6.828660696150925e-11</v>
+        <v>4.458093288320195e-16</v>
       </c>
       <c r="G13" t="n">
-        <v>-6.828641886836668e-11</v>
+        <v>-9.714667506989633e-22</v>
       </c>
       <c r="H13" t="n">
-        <v>-3.862868507645601e-11</v>
+        <v>9.326104496450015e-22</v>
       </c>
       <c r="I13" t="n">
-        <v>-9.092966050562929e-12</v>
+        <v>2.141328404866438e-27</v>
       </c>
       <c r="J13" t="n">
-        <v>2.734787184700931e-11</v>
+        <v>7.771726278103482e-22</v>
       </c>
       <c r="K13" t="n">
-        <v>-8.715238596914975e-26</v>
+        <v>-1.207146409970206e-11</v>
       </c>
       <c r="L13" t="n">
-        <v>-1.065837667222179e-21</v>
+        <v>-6.913053972440056e-20</v>
       </c>
       <c r="M13" t="n">
-        <v>-5.794339357851038e-22</v>
+        <v>7.178117670797212e-12</v>
       </c>
       <c r="N13" t="n">
-        <v>-6.981834875761937e-28</v>
+        <v>-9.599540615954022e-12</v>
       </c>
       <c r="O13" t="n">
-        <v>-4.766661924972722e-22</v>
+        <v>-8.779246611389223e-12</v>
       </c>
       <c r="P13" t="n">
-        <v>-4.472847828317725e-33</v>
+        <v>2.48604860623767e-23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-1.5756342512065e-16</v>
+        <v>-1.363247918779208e-20</v>
       </c>
       <c r="B14" t="n">
-        <v>-2.414290007734553e-11</v>
+        <v>-3.842194312588082e-23</v>
       </c>
       <c r="C14" t="n">
-        <v>-8.041775851746166e-17</v>
+        <v>1.96684543438495e-17</v>
       </c>
       <c r="D14" t="n">
-        <v>7.878977529051663e-17</v>
+        <v>-6.209438931723159e-18</v>
       </c>
       <c r="E14" t="n">
-        <v>-1.038105732383381e-17</v>
+        <v>-8.779236340784484e-12</v>
       </c>
       <c r="F14" t="n">
-        <v>2.731455399390334e-11</v>
+        <v>9.657168217908482e-12</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.731445555949354e-11</v>
+        <v>-5.796898387193339e-20</v>
       </c>
       <c r="H14" t="n">
-        <v>-7.29157315092532e-18</v>
+        <v>-2.219195522183423e-20</v>
       </c>
       <c r="I14" t="n">
-        <v>0.944137152813714</v>
+        <v>-1.609528543151388e-11</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1327032541270937</v>
+        <v>-1.931434255719504e-11</v>
       </c>
       <c r="K14" t="n">
-        <v>2.209214383758155e-16</v>
+        <v>3.048202111996052e-17</v>
       </c>
       <c r="L14" t="n">
-        <v>-1.09590350685046e-25</v>
+        <v>-2.127441337955986e-16</v>
       </c>
       <c r="M14" t="n">
-        <v>3.219057089704948e-11</v>
+        <v>-8.65273874625468e-16</v>
       </c>
       <c r="N14" t="n">
-        <v>2.759191791175612e-11</v>
+        <v>2.535015456704221e-16</v>
       </c>
       <c r="O14" t="n">
-        <v>-1.675666780433509e-25</v>
+        <v>3.232611405306137e-15</v>
       </c>
       <c r="P14" t="n">
-        <v>2.452460505825282e-22</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.931434253822951e-10</v>
+        <v>4.023897749873957e-12</v>
       </c>
       <c r="B15" t="n">
+        <v>-8.935451958260775e-34</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2.021477049285494e-16</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-1.048249412700043e-16</v>
+      </c>
+      <c r="E15" t="n">
         <v>-1</v>
       </c>
-      <c r="C15" t="n">
-        <v>-5.797682360548315e-16</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-2.271909548600767e-15</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1.457283827394942e-17</v>
-      </c>
       <c r="F15" t="n">
-        <v>-4.55242756308276e-11</v>
+        <v>-1.570680296142588e-15</v>
       </c>
       <c r="G15" t="n">
-        <v>-4.552440825531886e-11</v>
+        <v>-1.13985613885977e-21</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.219057089706281e-11</v>
+        <v>3.170345555754564e-31</v>
       </c>
       <c r="I15" t="n">
-        <v>-2.279430734335372e-11</v>
+        <v>9.326095690807819e-22</v>
       </c>
       <c r="J15" t="n">
-        <v>-3.203745108759551e-12</v>
+        <v>8.289862837575212e-22</v>
       </c>
       <c r="K15" t="n">
-        <v>3.328109496085297e-25</v>
+        <v>8.882880721229753e-22</v>
       </c>
       <c r="L15" t="n">
-        <v>-6.149074082706975e-22</v>
+        <v>1.207146409776064e-11</v>
       </c>
       <c r="M15" t="n">
-        <v>-7.77174641007935e-22</v>
+        <v>7.975790826044586e-12</v>
       </c>
       <c r="N15" t="n">
-        <v>-5.107147640916535e-22</v>
+        <v>-1.066638811050178e-11</v>
       </c>
       <c r="O15" t="n">
-        <v>9.948612767191988e-35</v>
+        <v>3.587011519156772e-21</v>
       </c>
       <c r="P15" t="n">
-        <v>-4.13683959236623e-33</v>
+        <v>8.779246608354961e-12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-9.110429739083297e-26</v>
+        <v>3.862625908880551e-12</v>
       </c>
       <c r="B16" t="n">
-        <v>1.589774002716592e-16</v>
+        <v>-7.920831019283158e-34</v>
       </c>
       <c r="C16" t="n">
-        <v>6.828548122608369e-11</v>
+        <v>3.194773389598348e-17</v>
       </c>
       <c r="D16" t="n">
-        <v>-6.828755107045754e-11</v>
+        <v>-2.381594983173658e-16</v>
       </c>
       <c r="E16" t="n">
-        <v>1.126734025035226e-16</v>
+        <v>-9.822805366194853e-16</v>
       </c>
       <c r="F16" t="n">
-        <v>0.70710805536802</v>
+        <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.7071055070027789</v>
+        <v>9.781508744603279e-31</v>
       </c>
       <c r="H16" t="n">
-        <v>3.743438718584211e-26</v>
+        <v>1.139856140506642e-21</v>
       </c>
       <c r="I16" t="n">
-        <v>-3.647085296111135e-11</v>
+        <v>9.714683009923193e-22</v>
       </c>
       <c r="J16" t="n">
-        <v>-5.126282407211175e-12</v>
+        <v>8.393486126241836e-22</v>
       </c>
       <c r="K16" t="n">
-        <v>-2.759191791175633e-11</v>
+        <v>-8.627754183637854e-22</v>
       </c>
       <c r="L16" t="n">
-        <v>3.431099875263232e-34</v>
+        <v>-3.955176453598527e-21</v>
       </c>
       <c r="M16" t="n">
-        <v>-8.260877303035707e-22</v>
+        <v>8.075010142429449e-12</v>
       </c>
       <c r="N16" t="n">
-        <v>-1.065839507667986e-21</v>
+        <v>1.316200083213747e-12</v>
       </c>
       <c r="O16" t="n">
-        <v>-6.695658445613472e-22</v>
+        <v>-1.073019029912856e-11</v>
       </c>
       <c r="P16" t="n">
-        <v>-5.4050651607276e-33</v>
+        <v>9.657171269116426e-12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.243479557629784e-20</v>
+        <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>-6.438114179409828e-11</v>
+        <v>3.707189766630389e-44</v>
       </c>
       <c r="C17" t="n">
-        <v>6.828764426041128e-11</v>
+        <v>-4.389623327864951e-12</v>
       </c>
       <c r="D17" t="n">
-        <v>6.828537506749272e-11</v>
+        <v>-4.198770128267268e-12</v>
       </c>
       <c r="E17" t="n">
-        <v>1.93143425382295e-10</v>
+        <v>4.023819818031322e-12</v>
       </c>
       <c r="F17" t="n">
-        <v>0.707105507002779</v>
+        <v>-3.862875931147207e-12</v>
       </c>
       <c r="G17" t="n">
-        <v>0.7071080553680201</v>
+        <v>1.055404632371026e-32</v>
       </c>
       <c r="H17" t="n">
-        <v>4.559432667379332e-21</v>
+        <v>-1.000542051913699e-32</v>
       </c>
       <c r="I17" t="n">
-        <v>2.897928656279906e-21</v>
+        <v>-8.93452432511236e-33</v>
       </c>
       <c r="J17" t="n">
-        <v>-2.227570613316149e-21</v>
+        <v>-7.856347481115003e-33</v>
       </c>
       <c r="K17" t="n">
-        <v>1.42746543255417e-21</v>
+        <v>7.028571994197634e-23</v>
       </c>
       <c r="L17" t="n">
-        <v>5.024271810181825e-32</v>
+        <v>-6.903515939756928e-23</v>
       </c>
       <c r="M17" t="n">
-        <v>3.832215787878858e-32</v>
+        <v>6.394251278974946e-17</v>
       </c>
       <c r="N17" t="n">
-        <v>3.750088912921917e-32</v>
+        <v>-3.226509235403771e-17</v>
       </c>
       <c r="O17" t="n">
-        <v>2.857597990731825e-32</v>
+        <v>5.510613654697584e-23</v>
       </c>
       <c r="P17" t="n">
-        <v>1.415430784746575e-43</v>
+        <v>-5.087355226303406e-23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>